<commit_message>
Finished up to the year 2015.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="301">
   <si>
     <t>variable</t>
   </si>
@@ -122,17 +122,68 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In subsequent years they no longer list the data source as BRFSS.</t>
+      <t xml:space="preserve">changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013, they no longer list the data source as BRFSS, but they start again in2014. In 2015, they list the source as the CDC Diabetes Interactive Atlas.</t>
     </r>
   </si>
   <si>
+    <t>food_environment_index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicator of access to healthy foods. 0 is worst and 10 is best. Unsure what numerator and denominator are. It is an index of factors which contribute to a healthy food environment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usda fea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USDA Food Environmental Atlas; Map the Meal Gap From Feeding America</t>
+  </si>
+  <si>
     <t>physical_inactivity</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage of adults ages 20 and older reporting no leisure time physical activity.</t>
   </si>
   <si>
-    <t xml:space="preserve">Starting in 2012, the listed source changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In subsequent years they no longer list the data source as BRFSS.</t>
+    <t xml:space="preserve">Starting in 2012, the listed source changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013,  they no longer list the data source as BRFSS, but they start again in 2014. In 2015, they list the source as the CDC DIabetes Interactive Atlas.</t>
+  </si>
+  <si>
+    <t>access_to_exercise_opportunities</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Percentage of the population with access to places for physical activity. Numerator is the number of people with access to exercise opportunities. Denominator is </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>presumably</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the number of people.</t>
+    </r>
+  </si>
+  <si>
+    <t>ogbb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OneSource Global Business Browser, Delorme map data, ESRI, &amp; US Census Tigerline Files</t>
   </si>
   <si>
     <t>binge_drinking</t>
@@ -147,7 +198,19 @@
     <t xml:space="preserve">Percent of adults that report excessive drinking in the past 30 days. Denominators reflect sample sizes of the survey.</t>
   </si>
   <si>
-    <t xml:space="preserve">In 2013, they define excessive drinking as adults who report heavy or binge drinking. It is unclear, as a result, how different this variable is from binge_drinking.</t>
+    <t xml:space="preserve">Starting in 2013, they define excessive drinking as adults who report heavy or binge drinking. It is unclear, as a result, how different this variable is from binge_drinking.</t>
+  </si>
+  <si>
+    <t>alcohol-impaired_driving_deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of driving deaths with alcohol involvement. Numerator is the total number of alcohol-impaired motor vehicle deaths. The denominator is the total number of motor vehicle deaths.</t>
+  </si>
+  <si>
+    <t>fars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatality Analysis Reporting System</t>
   </si>
   <si>
     <t>motor_vehicle_crash_deaths</t>
@@ -216,7 +279,31 @@
     <t xml:space="preserve">Number of primary care providers in patient care per person. The ratio value is the number of people per primary care provider in patient care (reciprocal). Numerator is the number of primary care providers in patient care. The denominator is the number of people.</t>
   </si>
   <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio in 2011, 2012, and 2013.</t>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2015.</t>
+  </si>
+  <si>
+    <t>dentists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of dentists per person. The ratio value is the number of people per dentist (reciprocal). Numerator is the number of dentists. Denominator is the number of people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_dentists to this variable and changed the stem value to ratio from 2012-2015.</t>
+  </si>
+  <si>
+    <t>mental_health_providers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of mental health providers per person. The ratio value is the number of people per mental health provider (reciprocal). Numerator is the number of mental health providers. Denominator is the number of people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cms npi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMS National Provider Identification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2015. Starting in 2014, the source of the variable changes to cms npi.</t>
   </si>
   <si>
     <t>preventable_hospital_stays</t>
@@ -261,7 +348,7 @@
     <t xml:space="preserve">national center for education statistics</t>
   </si>
   <si>
-    <t xml:space="preserve">State data sources used for Kentucky, New Hampshire, North Carolina, Pennsylvania, South Carolina, and Utah for the years 2010 and 2011. State data sources used for Alaska, Alabama, Arkansas, California, Connecticut, Florida, Hawaii, Idaho, Kentucky, Montana, North Dakota, New Jersey, Oklahoma, South Dakota, and Tennessee in 2012. Unclear in 2013 which states use which data source.</t>
+    <t xml:space="preserve">State data sources used for Kentucky, New Hampshire, North Carolina, Pennsylvania, South Carolina, and Utah for the years 2010 and 2011. State data sources used for Alaska, Alabama, Arkansas, California, Connecticut, Florida, Hawaii, Idaho, Kentucky, Montana, North Dakota, New Jersey, Oklahoma, South Dakota, and Tennessee in 2012. Unclear in 2013 which states use which data source. Starting in 2014, they mention NCES data is used to supplement data from data.gov.</t>
   </si>
   <si>
     <t>college_degrees</t>
@@ -306,10 +393,19 @@
     <t xml:space="preserve">small area income and poverty estimates</t>
   </si>
   <si>
+    <t>gini_coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gini coefficient of household income inequality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I changed this variable from income_inequality to gini_coefficient in 2010. This is to differentiate it from later versions of income_inequality which calculate income inequality differently.</t>
+  </si>
+  <si>
     <t>income_inequality</t>
   </si>
   <si>
-    <t xml:space="preserve">Gini coefficient of household income inequality.</t>
+    <t xml:space="preserve">Ratio of income at 80th percentile to income at the 20th percentile.</t>
   </si>
   <si>
     <t>inadequate_social_support</t>
@@ -327,10 +423,22 @@
     <t xml:space="preserve">children_in_single-parent_households </t>
   </si>
   <si>
-    <t xml:space="preserve">Percentage of all households with children that are single-parent households.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I believe in 2010 this measure (named single-parent_households) reflected the percentage of all households which were single-parent households. Starting in 2011 (I think), it changed to reflect the percentage of all households with children that are single-parent households. Documentation is unclear. Starting in 2012, I am more certain the variable changes to reflect the latter definition.</t>
+    <t xml:space="preserve">Percentage of all households with children that are single-parent households. Starting in 2014, they make the numerator and denominator explicit. The numerator is the number of children that live in single-parent households. The denominator is the number of children living in households.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I believe in 2010 this measure (named single-parent_households) reflected the percentage of all households which were single-parent households. Starting in 2011 (I think), it changed to reflect the percentage of all households with children that are single-parent households. Documentation is unclear. Starting in 2012, I am more certain the variable changes to reflect the latter definition.\</t>
+  </si>
+  <si>
+    <t>social_associations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of membership associations per 10,000 people. The numerator is the number of associations. </t>
+  </si>
+  <si>
+    <t>ccbp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">census county business patterns</t>
   </si>
   <si>
     <t>violent_crime</t>
@@ -348,25 +456,40 @@
     <t xml:space="preserve">State data sources used for Kentucky and Illinois in 2010 and just Illinois in 2011, 2012 and 2013.</t>
   </si>
   <si>
+    <t>injury_deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of deaths due to injury per 100,000 people. The numerator is the number of injury deaths.</t>
+  </si>
+  <si>
     <t>homicides</t>
   </si>
   <si>
     <t xml:space="preserve">Age-adjusted homicide rate per 100,000.</t>
   </si>
   <si>
+    <t>air_pollution-particulate_matter_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual number of days that the air quality was unhealthy due to fine particulate matter.</t>
+  </si>
+  <si>
+    <t>ephtn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental Public Health Tracking Network, EPA and CDC Wonder</t>
+  </si>
+  <si>
     <t>air_pollution_-_particulate_matter</t>
   </si>
   <si>
-    <t xml:space="preserve">Annual number of days that the air quality was unhealthy due to fine particulate matter.</t>
-  </si>
-  <si>
-    <t>ephtn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environmental Public Health Tracking Network, EPA and CDC Wonder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From 2010-2012, this variable used to be called air_pollution-particulate_matter_days. Starting in 2013, the name changed to the current entry. I updated the name from older releases to reflect the newer name.</t>
+    <t xml:space="preserve">Average daily amount of fine particulate matter in micrograms per cubic meter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdc wonder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDC wonder environmental data</t>
   </si>
   <si>
     <t>air_pollution-ozone_days</t>
@@ -378,7 +501,7 @@
     <t>drinking_water_violations</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent of population exposed to water exceeding a violation limit in the past year.</t>
+    <t xml:space="preserve">Percent of population exposed to water exceeding a violation limit in the past year. Numerator is the total number of people affected by a water violation. The denominator is the total number of people with access to public water.</t>
   </si>
   <si>
     <t>sdwis</t>
@@ -387,6 +510,30 @@
     <t xml:space="preserve">Safe Drinking Water Information System</t>
   </si>
   <si>
+    <t>severe_housing_problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of households with at least one of the following four housing problems: overcrowding, high housing costs, lack of kitchen, lack of plumbing.</t>
+  </si>
+  <si>
+    <t>chas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprehensive Housing Affordability Strategy</t>
+  </si>
+  <si>
+    <t>driving_alone_to_work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of labor force that drives alone. Unclear what numerator and denominator are. In 2014, they state the numerator is the number of people who drive alone to work, and the denominator is the number of workers in the labor force.</t>
+  </si>
+  <si>
+    <t>long_commute_-_driving_alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Among workers who commute in their vehicle alone, the percentage that commute more than 30 minutes. The denominator is the number of people who drive alone to work.</t>
+  </si>
+  <si>
     <t>access_to_healthy_foods</t>
   </si>
   <si>
@@ -408,9 +555,6 @@
     <t xml:space="preserve">Percent of people with limited access to health foods. Numerator is the total number of people with limited access to health foods.</t>
   </si>
   <si>
-    <t xml:space="preserve">usda fea</t>
-  </si>
-  <si>
     <t xml:space="preserve">USDA Food Environmental Atlas</t>
   </si>
   <si>
@@ -423,12 +567,6 @@
     <t xml:space="preserve">The number of recreational facilities per 100,000 people. Numerator is the total number of recreational facilities. The denominator is the total population.</t>
   </si>
   <si>
-    <t>ccbp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">census county business patterns</t>
-  </si>
-  <si>
     <t>fast_food_restaurants</t>
   </si>
   <si>
@@ -519,13 +657,13 @@
     <t xml:space="preserve">Percentage of adults ages 20 and older diagnosed with diabetes.</t>
   </si>
   <si>
-    <t>saoe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small area obesity estimates, CDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In 2013, the listed data source changed to the national center for chronic disease prevention and health promotion. This may or may not represent a real change in the data source.</t>
+    <t xml:space="preserve">saoe; nccdphp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small area obesity estimates, CDC; national center for chronic disease prevention and health promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2013, the listed data source changed to the national center for chronic disease prevention and health promotion. This may or may not represent a real change in the data source. In 2015, the source changed to the CDC Diabetes Interactive Atlas.</t>
   </si>
   <si>
     <t>hiv_prevalence</t>
@@ -540,27 +678,42 @@
     <t xml:space="preserve">No documentation available.</t>
   </si>
   <si>
-    <t xml:space="preserve">cdc wonder</t>
-  </si>
-  <si>
     <t xml:space="preserve">CDC Wonder and Mortality Data</t>
   </si>
   <si>
     <t>child_mortality</t>
   </si>
   <si>
+    <t>drug_poisoning_deaths</t>
+  </si>
+  <si>
+    <t>food_insecurity</t>
+  </si>
+  <si>
+    <t>mmg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map the meal gap</t>
+  </si>
+  <si>
     <t>infant_mortality</t>
   </si>
   <si>
-    <t>mental_health_providers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of mental health providers per person. The ratio value is the number of people per mental health provider (reciprocal). Numerator is the number of mental health providers. Denominator is the number of people.</t>
+    <t>hiw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">health indicators warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The listed source changed from CDC wonder data to hiw in 2014.</t>
   </si>
   <si>
     <t>health_care_costs</t>
   </si>
   <si>
+    <t xml:space="preserve">dartmouth atlas of health care</t>
+  </si>
+  <si>
     <t xml:space="preserve">In 2013, the listed data source changed to the Dartmouth Atlast of Health Care. This may or may not represent a real change in the data source.</t>
   </si>
   <si>
@@ -570,13 +723,10 @@
     <t>could_not_see_doctor_due_to_cost</t>
   </si>
   <si>
-    <t>dentists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of dentists per person. The ratio value is the number of people per dentist (reciprocal). Numerator is the number of dentists. Denominator is the number of people.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_dentists to this variable and changed the stem value to ratio in 2012 and 2013.</t>
+    <t>other_primary_care_providers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers_other_than_physicians to this variable and changed the stem value to ratio for years 2014-2015.</t>
   </si>
   <si>
     <t>median_household_income</t>
@@ -597,15 +747,12 @@
     <t xml:space="preserve">Percentage of  children in public schools eligible for free lunch.</t>
   </si>
   <si>
+    <t>nces</t>
+  </si>
+  <si>
     <t xml:space="preserve">In 2013, the listed data source changed to the national center for education statistics. This may or may not represent a real change in the data source.</t>
   </si>
   <si>
-    <t>driving_alone_to_work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of labor force that drives alone. Unclear what numerator and denominator are.</t>
-  </si>
-  <si>
     <t>access_to_parks</t>
   </si>
   <si>
@@ -729,7 +876,7 @@
     <t>cerebrovascular_disease_hospitalizations</t>
   </si>
   <si>
-    <t>inflicted_injury_hospitalizations</t>
+    <t>self-inflicted_injury_hospitalizations</t>
   </si>
   <si>
     <t>cancer_incidence</t>
@@ -811,6 +958,18 @@
   </si>
   <si>
     <t>population_growth</t>
+  </si>
+  <si>
+    <t>breastfeeding</t>
+  </si>
+  <si>
+    <t>influenza_immunizations_65+</t>
+  </si>
+  <si>
+    <t>cervical_cancer_screening</t>
+  </si>
+  <si>
+    <t>colon_cancer_screening</t>
   </si>
 </sst>
 </file>
@@ -1349,7 +1508,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -1358,11 +1517,11 @@
   <cols>
     <col bestFit="1" min="1" max="1" style="1" width="44.140625"/>
     <col customWidth="1" min="2" max="2" style="2" width="80.00390625"/>
-    <col bestFit="1" min="3" max="3" style="1" width="10.57421875"/>
+    <col bestFit="1" min="3" max="3" style="1" width="13.33203125"/>
     <col customWidth="1" min="4" max="4" style="2" width="37.57421875"/>
     <col customWidth="1" min="5" max="5" style="2" width="7.421875"/>
     <col customWidth="1" min="6" max="6" style="2" width="13.7109375"/>
-    <col customWidth="1" min="7" max="7" style="2" width="47.140625"/>
+    <col customWidth="1" min="7" max="7" style="2" width="65.28125"/>
     <col min="8" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
@@ -1509,203 +1668,200 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" ht="57">
-      <c r="A9" s="1" t="s">
+    <row r="9" ht="28.5">
+      <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" ht="57">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" ht="28.5">
-      <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" ht="57">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" ht="28.5">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" ht="28.5">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" ht="57">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" ht="42.75">
-      <c r="A14" s="1" t="s">
+      <c r="G13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="14" ht="57">
+      <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
+      <c r="B14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" ht="28.5">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" ht="28.5">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" ht="199.5">
-      <c r="A17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>52</v>
+      <c r="G16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" ht="28.5">
+      <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" ht="57">
-      <c r="A18" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    </row>
+    <row r="18" ht="28.5">
+      <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" ht="42.75">
+    </row>
+    <row r="19" ht="28.5">
       <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" ht="28.5">
+    <row r="20" ht="199.5">
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
@@ -1713,311 +1869,322 @@
         <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" ht="28.5">
+      <c r="G20" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" ht="57">
       <c r="A21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" ht="28.5">
+      <c r="G21" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" ht="57">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" ht="114">
+      <c r="G22" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" ht="57">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="G23" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" ht="28.5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" ht="42.75">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" ht="42.75">
+    <row r="25" ht="28.5">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" ht="57">
+    <row r="26" ht="28.5">
       <c r="A26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" ht="28.5">
       <c r="A27" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-    </row>
-    <row r="28" ht="28.5">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" ht="114">
       <c r="A28" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
+      <c r="G28" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="29" ht="28.5">
       <c r="A29" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" ht="28.5">
+    <row r="30" ht="42.75">
       <c r="A30" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" ht="114">
+    </row>
+    <row r="31" ht="42.75">
       <c r="A31" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="5" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="32" ht="28.5">
       <c r="A32" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" ht="28.5">
-      <c r="A33" s="1" t="s">
-        <v>102</v>
+    </row>
+    <row r="33" ht="42.75">
+      <c r="A33" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-    </row>
-    <row r="34" ht="71.25">
+      <c r="G33" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" ht="28.5">
       <c r="A34" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" ht="28.5">
       <c r="A35" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>107</v>
+        <v>13</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
     <row r="36" ht="28.5">
       <c r="A36" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-    </row>
-    <row r="37" ht="42.75">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" ht="114">
       <c r="A37" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="38" ht="57">
-      <c r="A38" s="1" t="s">
+    <row r="38" ht="114">
+      <c r="A38" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="6" t="s">
         <v>122</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2025,1577 +2192,2000 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="5" t="s">
-        <v>124</v>
-      </c>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" ht="28.5">
       <c r="A39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="40" ht="28.5">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>128</v>
+      <c r="C40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="2" t="s">
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" ht="28.5">
+      <c r="A41" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>133</v>
+        <v>9</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>134</v>
+        <v>10</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="s">
+    </row>
+    <row r="42" ht="71.25">
+      <c r="A42" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="s">
+    <row r="43" ht="71.25">
+      <c r="A43" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>134</v>
+      <c r="C43" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="s">
-        <v>139</v>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" ht="28.5">
+      <c r="A44" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>142</v>
+    </row>
+    <row r="45" ht="42.75">
+      <c r="A45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>134</v>
+    </row>
+    <row r="46" ht="28.5">
+      <c r="A46" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" ht="28.5">
-      <c r="A47" s="2" t="s">
-        <v>145</v>
+    </row>
+    <row r="47" ht="42.75">
+      <c r="A47" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>134</v>
+        <v>97</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>134</v>
+    <row r="48" ht="28.5">
+      <c r="A48" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49">
-      <c r="A49" s="2" t="s">
-        <v>149</v>
+    <row r="49" ht="42.75">
+      <c r="A49" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>133</v>
+        <v>156</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="s">
-        <v>151</v>
+      <c r="G49" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" ht="57">
+      <c r="A50" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="2" t="s">
-        <v>153</v>
+      <c r="G50" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" ht="28.5">
+      <c r="A51" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="s">
-        <v>155</v>
+    <row r="52" ht="28.5">
+      <c r="A52" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" ht="57">
-      <c r="A53" s="1" t="s">
-        <v>157</v>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="54" ht="28.5">
-      <c r="A54" s="1" t="s">
-        <v>162</v>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>41</v>
+        <v>171</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-    </row>
-    <row r="55" ht="28.5">
-      <c r="A55" s="6" t="s">
-        <v>164</v>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>167</v>
+        <v>175</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-    </row>
-    <row r="56" ht="28.5">
-      <c r="A56" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>167</v>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" ht="28.5">
-      <c r="A57" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>167</v>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-    </row>
-    <row r="58" ht="57">
-      <c r="A58" s="1" t="s">
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="D58" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" ht="57">
-      <c r="A59" s="1" t="s">
-        <v>172</v>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" ht="28.5">
+      <c r="A59" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>54</v>
+        <v>171</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" ht="57">
-      <c r="A60" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>48</v>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="8"/>
-    </row>
-    <row r="61" ht="57">
-      <c r="A61" s="1" t="s">
-        <v>175</v>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
-    </row>
-    <row r="62" ht="57">
-      <c r="A62" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>177</v>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-      <c r="G62" s="5" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="s">
-        <v>179</v>
+      <c r="A63" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-    </row>
-    <row r="64" ht="42.75">
-      <c r="A64" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>182</v>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>76</v>
+        <v>170</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>77</v>
+        <v>171</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65">
+    <row r="65" ht="57">
       <c r="A65" s="1" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>123</v>
+        <v>195</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="5" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" ht="28.5">
       <c r="A66" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>187</v>
+        <v>199</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
     <row r="67" ht="28.5">
-      <c r="A67" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>107</v>
+      <c r="A67" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
     </row>
     <row r="68" ht="28.5">
       <c r="A68" s="1" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
-    </row>
-    <row r="69" ht="71.25">
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" ht="28.5">
       <c r="A69" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>195</v>
+        <v>205</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
-      <c r="G69" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>165</v>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" ht="28.5">
+      <c r="A70" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="71">
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" ht="28.5">
       <c r="A71" s="1" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>198</v>
+        <v>139</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>203</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="72" ht="57">
       <c r="A72" s="1" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>198</v>
+        <v>65</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="G72" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="73" ht="57">
       <c r="A73" s="1" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>198</v>
+        <v>59</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="74">
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" ht="57">
       <c r="A74" s="1" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>198</v>
+        <v>13</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>165</v>
+        <v>14</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="75">
+    </row>
+    <row r="75" ht="57">
       <c r="A75" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>198</v>
+        <v>218</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="2" t="s">
-        <v>199</v>
+      <c r="G75" s="5" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>165</v>
+        <v>221</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>198</v>
+        <v>106</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="77">
+    </row>
+    <row r="77" ht="42.75">
       <c r="A77" s="1" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>165</v>
+        <v>223</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>198</v>
+        <v>96</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>165</v>
+        <v>97</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
-      <c r="G77" s="2" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>165</v>
+        <v>225</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>198</v>
+        <v>30</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
+        <v>162</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="G78" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="79" ht="28.5">
       <c r="A79" s="1" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>198</v>
+        <v>135</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="80">
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" ht="28.5">
       <c r="A80" s="1" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>165</v>
+        <v>230</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>198</v>
+        <v>231</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>165</v>
+        <v>232</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
-      <c r="G80" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="81">
+    </row>
+    <row r="81" ht="71.25">
       <c r="A81" s="1" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>165</v>
+        <v>234</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>198</v>
+        <v>122</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>165</v>
+        <v>235</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="2" t="s">
-        <v>208</v>
+      <c r="G81" s="5" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="6" t="s">
-        <v>222</v>
+      <c r="A91" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="5" t="s">
-        <v>223</v>
+      <c r="G91" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="94" ht="14.25">
-      <c r="A94" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>198</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>165</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
       <c r="G94" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="95" ht="14.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="95">
       <c r="A95" s="1" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="96" ht="14.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="96">
       <c r="A96" s="1" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="97" ht="14.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="97">
       <c r="A97" s="1" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="98" ht="14.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="98">
       <c r="A98" s="1" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="99" ht="14.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="99">
       <c r="A99" s="1" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="100" ht="14.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="100">
       <c r="A100" s="1" t="s">
-        <v>232</v>
+        <v>259</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="101" ht="14.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="101">
       <c r="A101" s="1" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="102" ht="14.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="102">
       <c r="A102" s="1" t="s">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="103" ht="14.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="103">
       <c r="A103" s="1" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
-      <c r="G103" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="104" ht="14.25">
+      <c r="G103" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="104">
       <c r="A104" s="1" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="105" ht="14.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="105">
       <c r="A105" s="1" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="106" ht="14.25">
       <c r="A106" s="1" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
+        <v>202</v>
+      </c>
       <c r="G106" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="107" ht="14.25">
       <c r="A107" s="1" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="1" t="s">
-        <v>240</v>
+        <v>268</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="109" ht="14.25">
-      <c r="A109" s="1" t="s">
-        <v>241</v>
+      <c r="A109" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="1" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="111" ht="14.25">
       <c r="A111" s="1" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="1" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="113" ht="14.25">
       <c r="A113" s="1" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="1" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="1" t="s">
-        <v>247</v>
+        <v>275</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="1" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="1" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="1" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="1" t="s">
-        <v>251</v>
+        <v>279</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="1" t="s">
-        <v>252</v>
+        <v>280</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="1" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="1" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="123" ht="14.25">
       <c r="A123" s="1" t="s">
-        <v>255</v>
+        <v>283</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="124" ht="14.25">
       <c r="A124" s="1" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2" t="s">
-        <v>216</v>
-      </c>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="125" ht="14.25">
+      <c r="A125" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="126" ht="14.25">
+      <c r="A126" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="127" ht="14.25">
+      <c r="A127" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="128" ht="14.25">
+      <c r="A128" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="129" ht="14.25">
+      <c r="A129" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="130" ht="14.25">
+      <c r="A130" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" ht="14.25">
+      <c r="A131" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="132" ht="14.25">
+      <c r="A132" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="133" ht="14.25">
+      <c r="A133" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="134" ht="14.25">
+      <c r="A134" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="135" ht="14.25">
+      <c r="A135" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="136" ht="14.25">
+      <c r="A136" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="137" ht="14.25">
+      <c r="A137" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="138" ht="14.25">
+      <c r="A138" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="139" ht="14.25">
+      <c r="A139" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="140" ht="14.25">
+      <c r="A140" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="141" ht="14.25">
+      <c r="A141" s="1"/>
+    </row>
+    <row r="142" ht="14.25">
+      <c r="A142" s="1"/>
+    </row>
+    <row r="143" ht="14.25">
+      <c r="A143" s="1"/>
+    </row>
+    <row r="144" ht="14.25">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" ht="14.25">
+      <c r="A145" s="1"/>
+    </row>
+    <row r="146" ht="14.25">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" ht="14.25">
+      <c r="A147" s="1"/>
+    </row>
+    <row r="148" ht="14.25">
+      <c r="A148" s="1"/>
+    </row>
+    <row r="149" ht="14.25">
+      <c r="A149" s="1"/>
+    </row>
+    <row r="150" ht="14.25">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" ht="14.25">
+      <c r="A151" s="1"/>
+    </row>
+    <row r="152" ht="14.25">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" ht="14.25">
+      <c r="A153" s="1"/>
+    </row>
+    <row r="154" ht="14.25">
+      <c r="A154" s="1"/>
+    </row>
+    <row r="155" ht="14.25">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" ht="14.25">
+      <c r="A156" s="1"/>
+    </row>
+    <row r="157" ht="14.25">
+      <c r="A157" s="1"/>
+    </row>
+    <row r="158" ht="14.25">
+      <c r="A158" s="1"/>
+    </row>
+    <row r="159" ht="14.25">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" ht="14.25">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="161" ht="14.25">
+      <c r="A161" s="1"/>
+    </row>
+    <row r="162" ht="14.25">
+      <c r="A162" s="1"/>
+    </row>
+    <row r="163" ht="14.25">
+      <c r="A163" s="1"/>
+    </row>
+    <row r="164" ht="14.25">
+      <c r="A164" s="1"/>
+    </row>
+    <row r="165" ht="14.25">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" ht="14.25">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="167" ht="14.25">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" ht="14.25">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169" ht="14.25">
+      <c r="A169" s="1"/>
+    </row>
+    <row r="170" ht="14.25">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" ht="14.25">
+      <c r="A171" s="1"/>
+    </row>
+    <row r="172" ht="14.25">
+      <c r="A172" s="1"/>
+    </row>
+    <row r="173" ht="14.25">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="174" ht="14.25">
+      <c r="A174" s="1"/>
+    </row>
+    <row r="175" ht="14.25">
+      <c r="A175" s="1"/>
+    </row>
+    <row r="176" ht="14.25">
+      <c r="A176" s="1"/>
+    </row>
+    <row r="177" ht="14.25">
+      <c r="A177" s="1"/>
+    </row>
+    <row r="178" ht="14.25">
+      <c r="A178" s="1"/>
+    </row>
+    <row r="179" ht="14.25">
+      <c r="A179" s="1"/>
+    </row>
+    <row r="180" ht="14.25">
+      <c r="A180" s="1"/>
+    </row>
+    <row r="181" ht="14.25">
+      <c r="A181" s="1"/>
+    </row>
+    <row r="182" ht="14.25">
+      <c r="A182" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Finished years 2016 and 2017.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="328">
   <si>
     <t>variable</t>
   </si>
@@ -122,7 +122,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013, they no longer list the data source as BRFSS, but they start again in2014. In 2015, they list the source as the CDC Diabetes Interactive Atlas.</t>
+      <t xml:space="preserve">changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013, they no longer list the data source as BRFSS, but they start again in 2014. In 2015, they list the source as the CDC Diabetes Interactive Atlas. From 2016-2017, some documentation lists the BRFSS while other documentation lists the CDC Diabetes Interactive Atlas.</t>
     </r>
   </si>
   <si>
@@ -144,7 +144,7 @@
     <t xml:space="preserve">Percentage of adults ages 20 and older reporting no leisure time physical activity.</t>
   </si>
   <si>
-    <t xml:space="preserve">Starting in 2012, the listed source changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013,  they no longer list the data source as BRFSS, but they start again in 2014. In 2015, they list the source as the CDC DIabetes Interactive Atlas.</t>
+    <t xml:space="preserve">Starting in 2012, the listed source changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013,  they no longer list the data source as BRFSS, but they start again in 2014. From 2015-2016, they list the source as the CDC DIabetes Interactive Atlas.</t>
   </si>
   <si>
     <t>access_to_exercise_opportunities</t>
@@ -210,7 +210,451 @@
     <t>fars</t>
   </si>
   <si>
-    <t xml:space="preserve">Fatality Analysis Reporting System</t>
+    <t xml:space="preserve">Fatality Analysis Reporting System. In 2016, they report the BRFSS as the source in some of the documentation, but I believe this is a mistake.</t>
+  </si>
+  <si>
+    <t>sexually_transmitted_infections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numer of chlamydia cases per 100,000 people. Numerator is the total number of chlamydia cases, and the denominator is the total population.</t>
+  </si>
+  <si>
+    <t>nchhstp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Center for Hepatitis, HIV, STD, and TB Prevention; CDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numerator and denominator are from different years in the 2010 release.</t>
+  </si>
+  <si>
+    <t>teen_births</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of teen births per 1000 teen females. Numerator is the number of teen births. The denominator is the number of teenage females. Teenagers are defined as 15 -19.</t>
+  </si>
+  <si>
+    <t>uninsured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of population under the age of 65 without health insurance.</t>
+  </si>
+  <si>
+    <t>sahie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small area health insurance estimates</t>
+  </si>
+  <si>
+    <t>primary_care_provider_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of primary care providers in patient care per 100,000 people. Ratio value is the number of people per primary care providers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hrsa arf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">health resources and services administration, area resource file (created from American Medical Association Master File and Census Population Estimates) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I transformed the primary_care_provider_rate_per_100000 into this variable and recoded the stem to be the raw value. Additionally, I recoded the ratio_of_population_to_primary_care_providers into this variable and recoded the stem to the ratio. Note this has a different variable name from other future versions of this variable despite ostensibly having the same data source (this variable name only exists in 2010). I would caution users when using this variable because I could not recreate the raw value/ratio values when using the given numerators and denominators. So it is unclear exactly what the creators of the data did to create this measure. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+  </si>
+  <si>
+    <t>primary_care_physicians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of primary care providers in patient care per person. The ratio value is the number of people per primary care provider in patient care (reciprocal). Numerator is the number of primary care providers in patient care. The denominator is the number of people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2017. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+  </si>
+  <si>
+    <t>dentists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of dentists per person. The ratio value is the number of people per dentist (reciprocal). Numerator is the number of dentists. Denominator is the number of people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_dentists to this variable and changed the stem value to ratio from 2012-2017. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+  </si>
+  <si>
+    <t>mental_health_providers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of mental health providers per person. The ratio value is the number of people per mental health provider (reciprocal). Numerator is the number of mental health providers. Denominator is the number of people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cms npi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMS National Provider Identification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2017. Starting in 2014, the source of the variable changes to cms npi. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+  </si>
+  <si>
+    <t>preventable_hospital_stays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of discharges for ambulatory care sensitive conditions per 1000 Medicare enrollees. The denominator is the number of Medicare enrollees. Can also be interpreted as a hospitalization rate.</t>
+  </si>
+  <si>
+    <t>dahc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicare claims &amp; Dartmouth Atlas of Health Care</t>
+  </si>
+  <si>
+    <t>diabetes_monitoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of Diabetic Medicare enrollees receiving HbA1c test. The denominator is the number of Diabetic Medicare enrollees.</t>
+  </si>
+  <si>
+    <t>mammography_screening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent female Medicare enrollees (age 67-69) having at least 1 mammogram in 2 yrs.</t>
+  </si>
+  <si>
+    <t>hospice_use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of chronically ill Medicare enrollees admitted to hospice in last 6 months of life. Denominator is unclear.</t>
+  </si>
+  <si>
+    <t>high_school_graduation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of ninth-grade cohort that graduates in 4 years. Denominator is the size of the freshman cohort. The numerator is the total number of diplomas awarded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nces; state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">national center for education statistics</t>
+  </si>
+  <si>
+    <t>edfacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State data sources used for Kentucky, New Hampshire, North Carolina, Pennsylvania, South Carolina, and Utah for the years 2010 and 2011. State data sources used for Alaska, Alabama, Arkansas, California, Connecticut, Florida, Hawaii, Idaho, Kentucky, Montana, North Dakota, New Jersey, Oklahoma, South Dakota, and Tennessee in 2012. Unclear in 2013 which states use which data source. Starting in 2014, they mention NCES data is used to supplement data from data.gov. Starting in 2016, the listed source is EDFacts.</t>
+  </si>
+  <si>
+    <t>college_degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of population ages 25 and older with at least a 4 year degree.</t>
+  </si>
+  <si>
+    <t>acs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">american community survey</t>
+  </si>
+  <si>
+    <t>some_college</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adults aged 25-44 with some post-secondary education. Denominator is the number of adults aged 25-44, and the numerator is the the number of adults aged 25-44 with some college education.</t>
+  </si>
+  <si>
+    <t>unemployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of population ages 16 and older that is unemployed but is seeking work. Numerator is the number of people aged 16 and older who are unemployed but are seeking work. The denominator is the size of the labor force.</t>
+  </si>
+  <si>
+    <t>laus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local area unemployment statistics</t>
+  </si>
+  <si>
+    <t>children_in_poverty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of children (under 18) living in poverty. Numerator is the number of children living in poverty.</t>
+  </si>
+  <si>
+    <t>saipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small area income and poverty estimates</t>
+  </si>
+  <si>
+    <t>gini_coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gini coefficient of household income inequality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I changed this variable from income_inequality to gini_coefficient in 2010. This is to differentiate it from later versions of income_inequality which calculate income inequality differently.</t>
+  </si>
+  <si>
+    <t>income_inequality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio of income at 80th percentile to income at the 20th percentile.</t>
+  </si>
+  <si>
+    <t>inadequate_social_support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of adults that reported not getting social/emotional support.  Numerators and denominators reflect sample sizes of the survey.</t>
+  </si>
+  <si>
+    <t>single-parent_households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of all households that are single parent households.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">children_in_single-parent_households </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of all households with children that are single-parent households. Starting in 2014, they make the numerator and denominator explicit. The numerator is the number of children that live in single-parent households. The denominator is the number of children living in households.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I believe in 2010 this measure (named single-parent_households) reflected the percentage of all households which were single-parent households. Starting in 2011 (I think), it changed to reflect the percentage of all households with children that are single-parent households. Documentation is unclear. Starting in 2012, I am more certain the variable changes to reflect the latter definition.</t>
+  </si>
+  <si>
+    <t>social_associations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of membership associations per 10,000 people. The numerator is the number of associations. </t>
+  </si>
+  <si>
+    <t>ccbp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">census county business patterns</t>
+  </si>
+  <si>
+    <t>violent_crime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of violent crimes per 100,000 individuals. Numerator is the number of reported violent crimes to the police. The denominator is the total population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ucr; state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniform Crime Reports, FBI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State data sources used for Kentucky and Illinois in 2010 and just Illinois in 2011, 2012 and 2013.</t>
+  </si>
+  <si>
+    <t>injury_deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of deaths due to injury per 100,000 people. The numerator is the number of injury deaths.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nchs; cdc wonder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">national center for health statistics, vital statistics; CDC wonder mortality data</t>
+  </si>
+  <si>
+    <t>air_pollution-particulate_matter_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual number of days that the air quality was unhealthy due to fine particulate matter.</t>
+  </si>
+  <si>
+    <t>ephtn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental Public Health Tracking Network, EPA and CDC Wonder</t>
+  </si>
+  <si>
+    <t>air_pollution_-_particulate_matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average daily amount of fine particulate matter in micrograms per cubic meter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdc wonder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDC wonder environmental data</t>
+  </si>
+  <si>
+    <t>air_pollution-ozone_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual number of days that the air quality was unhealthy due to ozone.</t>
+  </si>
+  <si>
+    <t>drinking_water_violations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of population exposed to water exceeding a violation limit in the past year. Numerator is the total number of people affected by a water violation. The denominator is the total number of people with access to public water.</t>
+  </si>
+  <si>
+    <t>sdwis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safe Drinking Water Information System</t>
+  </si>
+  <si>
+    <t>drinking_water_violations_bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the county level, binary value indicating whether or not the count was exposed to a drinking water violations. 1 = Yes, 0 = No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I rename this variable for the years 2016 to differentiate it from previous years' measure of drinking_water_violations because previous years measured this variable differently. </t>
+  </si>
+  <si>
+    <t>severe_housing_problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of households with at least one of the following four housing problems: overcrowding, high housing costs, lack of kitchen, lack of plumbing.</t>
+  </si>
+  <si>
+    <t>chas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprehensive Housing Affordability Strategy</t>
+  </si>
+  <si>
+    <t>driving_alone_to_work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of labor force that drives alone. Unclear what numerator and denominator are. In 2014, they state the numerator is the number of people who drive alone to work, and the denominator is the number of workers in the labor force.</t>
+  </si>
+  <si>
+    <t>long_commute_-_driving_alone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Among workers who commute in their vehicle alone, the percentage that commute more than 30 minutes. The denominator is the number of people who drive alone to work.</t>
+  </si>
+  <si>
+    <t>access_to_healthy_foods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of zip codes with a healthy food outlet. Numerator is the number of zip codes with a healthy food outlet. The denominator is the number of zip codes.</t>
+  </si>
+  <si>
+    <t>czcbp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">census zip code business patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healthy food outlets include grocery stores (NAICS 445110) with &gt; 4 employees and produce stands or farmers’ markets (NAICS 445230).</t>
+  </si>
+  <si>
+    <t>access_to_recreational_facilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of recreational facilities per 100,000 people. Numerator is the total number of recreational facilities. The denominator is the total population.</t>
+  </si>
+  <si>
+    <t>fast_food_restaurants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of restaurants that are fast food restaurants. Numerator is the number of fast food restaurants, and the denominator is the number of restaurants.</t>
+  </si>
+  <si>
+    <t>premature_age-adjusted_mortality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No documentation available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDC Wonder and Mortality Data</t>
+  </si>
+  <si>
+    <t>child_mortality</t>
+  </si>
+  <si>
+    <t>infant_mortality</t>
+  </si>
+  <si>
+    <t>hiw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">health indicators warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The listed source changed from CDC wonder data to hiw in 2014.</t>
+  </si>
+  <si>
+    <t>frequent_physical_distress</t>
+  </si>
+  <si>
+    <t>frequent_mental_distress</t>
+  </si>
+  <si>
+    <t>diabetes_prevalence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of adults ages 20 and older diagnosed with diabetes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saoe; nccdphp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small area obesity estimates, CDC; national center for chronic disease prevention and health promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdc dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdc diabetes interactive atlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2013, the listed data source changed to the national center for chronic disease prevention and health promotion. This may or may not represent a real change in the data source. In 2015, the source changed to the CDC Diabetes Interactive Atlas.</t>
+  </si>
+  <si>
+    <t>hiv_prevalence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of positive screened individuals for HIV per 100,000 people. Denominator is the total population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hiv nss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">national hiv surveillance system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2016, the listed sourced changed to the National HIV Surveillance system.</t>
+  </si>
+  <si>
+    <t>food_insecurity</t>
+  </si>
+  <si>
+    <t>mmg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map the meal gap</t>
+  </si>
+  <si>
+    <t>limited_access_to_healthy_foods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of people with limited access to health foods. Numerator is the total number of people with limited access to health foods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USDA Food Environmental Atlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are definied as having limited access to health foods if you live in poverty and are more than 1 or 10 miles from a grocery store (?). From the documentation, seems a bit confusing.</t>
+  </si>
+  <si>
+    <t>drug_overdose_deaths</t>
+  </si>
+  <si>
+    <t>drug_overdose_deaths_-_modeled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the county level, values correspond to numeric codes which reflect modeled interval rates of drug overdose deaths per 100,000 people. The numeric codes are as follows:1 (0 - 2); 2 (2.1 - 4); 3 (4.1 - 6); 4 (6.1 - 8); 5 (8.1 - 10); 6 (10.1 - 12); 7 (12.1 - 14); 8 (14.1 - 16); 9 (16.1 - 18); 10 (18.1 - 20); 11 (&gt; 20)</t>
   </si>
   <si>
     <t>motor_vehicle_crash_deaths</t>
@@ -219,25 +663,10 @@
     <t xml:space="preserve">Crude motor-vehicle related mortality rate per 100,000 population. Numerator is the total number of motor vehicle-related deaths.</t>
   </si>
   <si>
-    <t>sexually_transmitted_infections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numer of chlamydia cases per 100,000 people. Numerator is the total number of chlamydia cases, and the denominator is the total population.</t>
-  </si>
-  <si>
-    <t>nchhstp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Center for Hepatitis, HIV, STD, and TB Prevention; CDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerator and denominator are from different years in the 2010 release.</t>
-  </si>
-  <si>
-    <t>teen_births</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of teen births per 1000 teen females. Numerator is the number of teen birth counts. The denominator is the number of teenage females. Teenagers are defined as 15 -19.</t>
+    <t xml:space="preserve">national center for health statistics, vital statistics, CDC Wonder and Mortality Data</t>
+  </si>
+  <si>
+    <t>insufficient_sleep</t>
   </si>
   <si>
     <t>uninsured_adults</t>
@@ -246,220 +675,61 @@
     <t xml:space="preserve">Percentage of adults (18-64) without health insurance .</t>
   </si>
   <si>
-    <t>sahie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">small area health insurance estimates</t>
-  </si>
-  <si>
-    <t>uninsured</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of population under the age of 65 without health insurance.</t>
-  </si>
-  <si>
-    <t>primary_care_provider_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of primary care providers in patient care per 100,000 people. Ratio value is the number of people per primary care providers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hrsa arf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health resources and services administration, area resource file (created from American Medical Association Master File and Census Population Estimates) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I transformed the primary_care_provider_rate_per_100000 into this variable and recoded the stem to be the raw value. Additionally, I recoded the ratio_of_population_to_primary_care_providers into this variable and recoded the stem to the ratio. Note this has a different variable name from other future versions of this variable despite ostensibly having the same data source (this variable name only exists in 2010). I would caution users when using this variable because I could not recreate the raw value/ratio values when using the given numerators and denominators. So it is unclear exactly what the creators of the data did to create this measure.</t>
-  </si>
-  <si>
-    <t>primary_care_physicians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of primary care providers in patient care per person. The ratio value is the number of people per primary care provider in patient care (reciprocal). Numerator is the number of primary care providers in patient care. The denominator is the number of people.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2015.</t>
-  </si>
-  <si>
-    <t>dentists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of dentists per person. The ratio value is the number of people per dentist (reciprocal). Numerator is the number of dentists. Denominator is the number of people.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_dentists to this variable and changed the stem value to ratio from 2012-2015.</t>
-  </si>
-  <si>
-    <t>mental_health_providers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of mental health providers per person. The ratio value is the number of people per mental health provider (reciprocal). Numerator is the number of mental health providers. Denominator is the number of people.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cms npi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMS National Provider Identification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2015. Starting in 2014, the source of the variable changes to cms npi.</t>
-  </si>
-  <si>
-    <t>preventable_hospital_stays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of discharges for ambulatory care sensitive conditions per 1000 Medicare enrollees. The denominator is the number of Medicare enrollees. Can also be interpreted as a hospitalization rate.</t>
-  </si>
-  <si>
-    <t>dahc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicare claims &amp; Dartmouth Atlas of Health Care</t>
-  </si>
-  <si>
-    <t>diabetes_monitoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of Diabetic Medicare enrollees receiving HbA1c test. The denominator is the number of Diabetic Medicare enrollees.</t>
-  </si>
-  <si>
-    <t>mammography_screening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent female Medicare enrollees (age 67-69) having at least 1 mammogram in 2 yrs.</t>
-  </si>
-  <si>
-    <t>hospice_use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of chronically ill Medicare enrollees admitted to hospice in last 6 months of life. Denominator is unclear.</t>
-  </si>
-  <si>
-    <t>high_school_graduation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of ninth-grade cohort that graduates in 4 years. Denominator is the size of the freshman cohort. The numerator is the total number of diplomas awarded.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nces; state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">national center for education statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State data sources used for Kentucky, New Hampshire, North Carolina, Pennsylvania, South Carolina, and Utah for the years 2010 and 2011. State data sources used for Alaska, Alabama, Arkansas, California, Connecticut, Florida, Hawaii, Idaho, Kentucky, Montana, North Dakota, New Jersey, Oklahoma, South Dakota, and Tennessee in 2012. Unclear in 2013 which states use which data source. Starting in 2014, they mention NCES data is used to supplement data from data.gov.</t>
-  </si>
-  <si>
-    <t>college_degrees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of population ages 25 and older with at least a 4 year degree.</t>
-  </si>
-  <si>
-    <t>acs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">american community survey</t>
-  </si>
-  <si>
-    <t>some_college</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adults aged 25-44 with some post-secondary education. Denominator is the number of adults aged 25-44, and the numerator is the the number of adults aged 25-44 with some college education.</t>
-  </si>
-  <si>
-    <t>unemployment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of population ages 16 and older that is unemployed but is seeking work. Numerator is the number of people aged 16 and older who are unemployed but are seeking work. The denominator is the size of the labor force.</t>
-  </si>
-  <si>
-    <t>laus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">local area unemployment statistics</t>
-  </si>
-  <si>
-    <t>children_in_poverty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of children (under 18) living in poverty. Numerator is the number of children living in poverty.</t>
-  </si>
-  <si>
-    <t>saipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">small area income and poverty estimates</t>
-  </si>
-  <si>
-    <t>gini_coefficient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gini coefficient of household income inequality.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I changed this variable from income_inequality to gini_coefficient in 2010. This is to differentiate it from later versions of income_inequality which calculate income inequality differently.</t>
-  </si>
-  <si>
-    <t>income_inequality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio of income at 80th percentile to income at the 20th percentile.</t>
-  </si>
-  <si>
-    <t>inadequate_social_support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of adults that reported not getting social/emotional support.  Numerators and denominators reflect sample sizes of the survey.</t>
-  </si>
-  <si>
-    <t>single-parent_households</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of all households that are single parent households.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">children_in_single-parent_households </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of all households with children that are single-parent households. Starting in 2014, they make the numerator and denominator explicit. The numerator is the number of children that live in single-parent households. The denominator is the number of children living in households.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I believe in 2010 this measure (named single-parent_households) reflected the percentage of all households which were single-parent households. Starting in 2011 (I think), it changed to reflect the percentage of all households with children that are single-parent households. Documentation is unclear. Starting in 2012, I am more certain the variable changes to reflect the latter definition.\</t>
-  </si>
-  <si>
-    <t>social_associations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of membership associations per 10,000 people. The numerator is the number of associations. </t>
-  </si>
-  <si>
-    <t>ccbp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">census county business patterns</t>
-  </si>
-  <si>
-    <t>violent_crime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of violent crimes per 100,000 individuals. Numerator is the number of reported violent crimes to the police. The denominator is the total population.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ucr; state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uniform Crime Reports, FBI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State data sources used for Kentucky and Illinois in 2010 and just Illinois in 2011, 2012 and 2013.</t>
-  </si>
-  <si>
-    <t>injury_deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of deaths due to injury per 100,000 people. The numerator is the number of injury deaths.</t>
+    <t>uninsured_children</t>
+  </si>
+  <si>
+    <t>health_care_costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dartmouth atlas of health care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2013, the listed data source changed to the Dartmouth Atlast of Health Care. This may or may not represent a real change in the data source.</t>
+  </si>
+  <si>
+    <t>other_primary_care_providers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers_other_than_physicians to this variable and changed the stem value to ratio for years 2014-2017. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+  </si>
+  <si>
+    <t>disconnected_youth</t>
+  </si>
+  <si>
+    <t>moa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measure of america</t>
+  </si>
+  <si>
+    <t>median_household_income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median household income.</t>
+  </si>
+  <si>
+    <t>children_eligible_for_free_lunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of  children in public schools eligible for free lunch.</t>
+  </si>
+  <si>
+    <t>nces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2013, the listed data source changed to the national center for education statistics. This may or may not represent a real change in the data source. </t>
+  </si>
+  <si>
+    <t>children_eligible_for_free_or_reduced_price_lunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 2011-2016, this variable was called children_eligible_for_free_lunch. In 2017, it changed to children_eligible_for_free_or_reduced_price_lunch. It is unclear how, if at all, the variable changed though. The only indication we have of a change in the variable measurment is in 2013, the listed data source changed to the national center for education statistics.</t>
+  </si>
+  <si>
+    <t>residential_segregation_-_black/white</t>
+  </si>
+  <si>
+    <t>residential_segregation_-_non-white/white</t>
   </si>
   <si>
     <t>homicides</t>
@@ -468,109 +738,10 @@
     <t xml:space="preserve">Age-adjusted homicide rate per 100,000.</t>
   </si>
   <si>
-    <t>air_pollution-particulate_matter_days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual number of days that the air quality was unhealthy due to fine particulate matter.</t>
-  </si>
-  <si>
-    <t>ephtn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environmental Public Health Tracking Network, EPA and CDC Wonder</t>
-  </si>
-  <si>
-    <t>air_pollution_-_particulate_matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average daily amount of fine particulate matter in micrograms per cubic meter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cdc wonder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDC wonder environmental data</t>
-  </si>
-  <si>
-    <t>air_pollution-ozone_days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual number of days that the air quality was unhealthy due to ozone.</t>
-  </si>
-  <si>
-    <t>drinking_water_violations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of population exposed to water exceeding a violation limit in the past year. Numerator is the total number of people affected by a water violation. The denominator is the total number of people with access to public water.</t>
-  </si>
-  <si>
-    <t>sdwis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safe Drinking Water Information System</t>
-  </si>
-  <si>
-    <t>severe_housing_problems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of households with at least one of the following four housing problems: overcrowding, high housing costs, lack of kitchen, lack of plumbing.</t>
-  </si>
-  <si>
-    <t>chas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comprehensive Housing Affordability Strategy</t>
-  </si>
-  <si>
-    <t>driving_alone_to_work</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of labor force that drives alone. Unclear what numerator and denominator are. In 2014, they state the numerator is the number of people who drive alone to work, and the denominator is the number of workers in the labor force.</t>
-  </si>
-  <si>
-    <t>long_commute_-_driving_alone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Among workers who commute in their vehicle alone, the percentage that commute more than 30 minutes. The denominator is the number of people who drive alone to work.</t>
-  </si>
-  <si>
-    <t>access_to_healthy_foods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of zip codes with a healthy food outlet. Numerator is the number of zip codes with a healthy food outlet. The denominator is the number of zip codes.</t>
-  </si>
-  <si>
-    <t>czcbp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">census zip code business patterns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Healthy food outlets include grocery stores (NAICS 445110) with &gt; 4 employees and produce stands or farmers’ markets (NAICS 445230).</t>
-  </si>
-  <si>
-    <t>limited_access_to_healthy_foods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of people with limited access to health foods. Numerator is the total number of people with limited access to health foods.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USDA Food Environmental Atlas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You are definied as having limited access to health foods if you live in poverty and are more than 1 or 10 miles from a grocery store (?). From the documentation, seems a bit confusing.</t>
-  </si>
-  <si>
-    <t>access_to_recreational_facilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of recreational facilities per 100,000 people. Numerator is the total number of recreational facilities. The denominator is the total population.</t>
-  </si>
-  <si>
-    <t>fast_food_restaurants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of restaurants that are fast food restaurants. Numerator is the number of fast food restaurants, and the denominator is the number of restaurants.</t>
+    <t xml:space="preserve">In 2016, the source changed to CDC Wonder mortality data. It is unclear if this represents a real change in the data source.</t>
+  </si>
+  <si>
+    <t>firearm_fatalities</t>
   </si>
   <si>
     <t>population</t>
@@ -651,106 +822,16 @@
     <t xml:space="preserve">Percentage of total population that lives in rural areas.</t>
   </si>
   <si>
-    <t>diabetes_prevalence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of adults ages 20 and older diagnosed with diabetes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saoe; nccdphp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small area obesity estimates, CDC; national center for chronic disease prevention and health promotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In 2013, the listed data source changed to the national center for chronic disease prevention and health promotion. This may or may not represent a real change in the data source. In 2015, the source changed to the CDC Diabetes Interactive Atlas.</t>
-  </si>
-  <si>
-    <t>hiv_prevalence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of positive screened individuals for HIV per 100,000 people. Denominator is the total population.</t>
-  </si>
-  <si>
-    <t>premature_age-adjusted_mortality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No documentation available.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDC Wonder and Mortality Data</t>
-  </si>
-  <si>
-    <t>child_mortality</t>
-  </si>
-  <si>
     <t>drug_poisoning_deaths</t>
   </si>
   <si>
-    <t>food_insecurity</t>
-  </si>
-  <si>
-    <t>mmg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">map the meal gap</t>
-  </si>
-  <si>
-    <t>infant_mortality</t>
-  </si>
-  <si>
-    <t>hiw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health indicators warehouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The listed source changed from CDC wonder data to hiw in 2014.</t>
-  </si>
-  <si>
-    <t>health_care_costs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dartmouth atlas of health care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In 2013, the listed data source changed to the Dartmouth Atlast of Health Care. This may or may not represent a real change in the data source.</t>
-  </si>
-  <si>
-    <t>uninsured_children</t>
-  </si>
-  <si>
     <t>could_not_see_doctor_due_to_cost</t>
   </si>
   <si>
-    <t>other_primary_care_providers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers_other_than_physicians to this variable and changed the stem value to ratio for years 2014-2015.</t>
-  </si>
-  <si>
-    <t>median_household_income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Median household income.</t>
-  </si>
-  <si>
     <t>high_housing_costs</t>
   </si>
   <si>
     <t xml:space="preserve">% of households with high housing costs. Numerator is the total number of households with high housing costs. The denominator is the total number of households.</t>
-  </si>
-  <si>
-    <t>children_eligible_for_free_lunch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of  children in public schools eligible for free lunch.</t>
-  </si>
-  <si>
-    <t>nces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In 2013, the listed data source changed to the national center for education statistics. This may or may not represent a real change in the data source.</t>
   </si>
   <si>
     <t>access_to_parks</t>
@@ -1011,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1030,9 +1111,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1508,18 +1586,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" style="1" width="44.140625"/>
+    <col bestFit="1" min="1" max="1" style="1" width="44.90234375"/>
     <col customWidth="1" min="2" max="2" style="2" width="80.00390625"/>
     <col bestFit="1" min="3" max="3" style="1" width="13.33203125"/>
     <col customWidth="1" min="4" max="4" style="2" width="37.57421875"/>
-    <col customWidth="1" min="5" max="5" style="2" width="7.421875"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="2" width="7.76171875"/>
     <col customWidth="1" min="6" max="6" style="2" width="13.7109375"/>
     <col customWidth="1" min="7" max="7" style="2" width="65.28125"/>
     <col min="8" max="16384" style="1" width="9.140625"/>
@@ -1645,7 +1723,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" ht="57">
+    <row r="8" ht="85.5">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1669,21 +1747,21 @@
       </c>
     </row>
     <row r="9" ht="28.5">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" ht="57">
       <c r="A10" s="1" t="s">
@@ -1708,22 +1786,22 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" ht="57">
-      <c r="A11" s="6" t="s">
+    <row r="11" ht="42.75">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" ht="28.5">
       <c r="A12" s="1" t="s">
@@ -1742,7 +1820,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" ht="57">
+    <row r="13" ht="42.75">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -1757,18 +1835,18 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" ht="57">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1776,7 +1854,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" ht="28.5">
       <c r="A15" s="1" t="s">
@@ -1786,32 +1864,32 @@
         <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" ht="28.5">
       <c r="A16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="17" ht="28.5">
       <c r="A17" s="1" t="s">
@@ -1821,138 +1899,138 @@
         <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" ht="28.5">
+    <row r="18" ht="199.5">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" ht="28.5">
+      <c r="G18" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" ht="99.75">
       <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" ht="199.5">
+      <c r="G19" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" ht="85.5">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" ht="57">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" ht="99.75">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G21" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" ht="57">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" ht="42.75">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" ht="57">
+    </row>
+    <row r="23" ht="28.5">
       <c r="A23" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" ht="28.5">
+      <c r="A24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="D24" s="2" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="24" ht="42.75">
-      <c r="A24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1965,2134 +2043,2320 @@
         <v>84</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-    </row>
-    <row r="26" ht="28.5">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" ht="114">
       <c r="A26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="27" ht="28.5">
       <c r="A27" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" ht="114">
+    </row>
+    <row r="28" ht="42.75">
       <c r="A28" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" ht="28.5">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" ht="42.75">
       <c r="A29" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" ht="42.75">
+    <row r="30" ht="28.5">
       <c r="A30" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
     <row r="31" ht="42.75">
       <c r="A31" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="32" ht="28.5">
       <c r="A32" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-    </row>
-    <row r="33" ht="42.75">
-      <c r="A33" s="6" t="s">
-        <v>108</v>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" ht="28.5">
+      <c r="A33" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="5" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="34" ht="28.5">
-      <c r="A34" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>97</v>
+      <c r="B34" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" ht="28.5">
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" ht="85.5">
       <c r="A35" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
+      <c r="G35" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="36" ht="28.5">
       <c r="A36" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" ht="114">
+    <row r="37" ht="28.5">
       <c r="A37" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" ht="114">
-      <c r="A38" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>123</v>
+      <c r="G37" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" ht="28.5">
+      <c r="A38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="5"/>
+      <c r="G38" s="2"/>
     </row>
     <row r="39" ht="28.5">
       <c r="A39" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" ht="28.5">
-      <c r="A40" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>10</v>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" ht="71.25">
+      <c r="A40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="7"/>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" ht="28.5">
       <c r="A41" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" ht="71.25">
-      <c r="A42" s="6" t="s">
-        <v>133</v>
+    <row r="42" ht="42.75">
+      <c r="A42" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" ht="71.25">
+    </row>
+    <row r="43" ht="42.75">
       <c r="A43" s="6" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>140</v>
+        <v>145</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="7"/>
+      <c r="G43" s="5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="44" ht="28.5">
       <c r="A44" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
     <row r="45" ht="42.75">
       <c r="A45" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>144</v>
+        <v>151</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
     </row>
     <row r="46" ht="28.5">
       <c r="A46" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>150</v>
+        <v>153</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-    </row>
-    <row r="47" ht="42.75">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" ht="28.5">
       <c r="A47" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>96</v>
+        <v>157</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>97</v>
+        <v>158</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="G47" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="48" ht="28.5">
-      <c r="A48" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>97</v>
+      <c r="A48" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-    </row>
-    <row r="49" ht="42.75">
+    </row>
+    <row r="49" ht="28.5">
       <c r="A49" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>156</v>
+        <v>162</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="50" ht="57">
+    </row>
+    <row r="50" ht="28.5">
       <c r="A50" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="5" t="s">
-        <v>163</v>
-      </c>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" ht="28.5">
       <c r="A51" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-    </row>
-    <row r="52" ht="28.5">
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" ht="42.75">
       <c r="A52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="F52" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="53" ht="28.5">
+      <c r="A53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B54" s="2" t="s">
+    <row r="54" ht="28.5">
+      <c r="A54" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>171</v>
+      <c r="B54" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55">
-      <c r="A55" s="2" t="s">
+    <row r="55" ht="57">
+      <c r="A55" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>175</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" ht="42.75">
+      <c r="A56" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="2" t="s">
-        <v>178</v>
+        <v>51</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" ht="28.5">
+      <c r="A57" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58">
-      <c r="A58" s="2" t="s">
-        <v>180</v>
+    <row r="58" ht="42.75">
+      <c r="A58" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>170</v>
+        <v>30</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
+      <c r="G58" s="2" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="59" ht="28.5">
-      <c r="A59" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>171</v>
+      <c r="A59" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60">
-      <c r="A60" s="2" t="s">
-        <v>184</v>
+    <row r="60" ht="57">
+      <c r="A60" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="2" t="s">
-        <v>186</v>
+      <c r="G60" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" ht="28.5">
+      <c r="A61" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>171</v>
+        <v>197</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>97</v>
+    <row r="62" ht="28.5">
+      <c r="A62" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="2" t="s">
-        <v>190</v>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" ht="28.5">
+      <c r="A63" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>170</v>
+        <v>57</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>171</v>
+        <v>58</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="2" t="s">
-        <v>192</v>
+    </row>
+    <row r="64" ht="28.5">
+      <c r="A64" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>170</v>
+        <v>57</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>171</v>
+        <v>58</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-    </row>
-    <row r="65" ht="57">
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" ht="28.5">
       <c r="A65" s="1" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="5" t="s">
-        <v>198</v>
+        <v>165</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="66" ht="28.5">
       <c r="A66" s="1" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
+      <c r="G66" s="5" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="67" ht="28.5">
       <c r="A67" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
+      <c r="G67" s="7"/>
     </row>
     <row r="68" ht="28.5">
       <c r="A68" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" ht="28.5">
-      <c r="A69" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
+      <c r="A69" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="70" ht="28.5">
-      <c r="A70" s="6" t="s">
-        <v>206</v>
+      <c r="A70" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>208</v>
+        <v>88</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
+      <c r="G70" s="5" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="71" ht="28.5">
       <c r="A71" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="72" ht="57">
+        <v>219</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" ht="28.5">
       <c r="A72" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="73" ht="57">
+        <v>220</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" ht="28.5">
       <c r="A73" s="1" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-    </row>
-    <row r="74" ht="57">
+        <v>10</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="74" ht="28.5">
       <c r="A74" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" ht="57">
-      <c r="A75" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>76</v>
+        <v>224</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>77</v>
+        <v>228</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="5" t="s">
-        <v>219</v>
-      </c>
+      <c r="G75" s="2"/>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="s">
-        <v>220</v>
+      <c r="A76" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>106</v>
+        <v>227</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>107</v>
+        <v>228</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
-    </row>
-    <row r="77" ht="42.75">
-      <c r="A77" s="1" t="s">
-        <v>222</v>
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>96</v>
+        <v>227</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>97</v>
+        <v>228</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="s">
-        <v>224</v>
+      <c r="A78" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G78" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="79" ht="28.5">
-      <c r="A79" s="1" t="s">
+      <c r="D79" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" ht="28.5">
-      <c r="A80" s="1" t="s">
-        <v>229</v>
+    <row r="80">
+      <c r="A80" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
-    </row>
-    <row r="81" ht="71.25">
-      <c r="A81" s="1" t="s">
-        <v>233</v>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" ht="28.5">
+      <c r="A81" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="5" t="s">
-        <v>236</v>
-      </c>
+      <c r="G81" s="2"/>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="s">
-        <v>237</v>
+      <c r="A82" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
-      <c r="G82" s="2" t="s">
-        <v>239</v>
-      </c>
+      <c r="G82" s="2"/>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="s">
-        <v>240</v>
+      <c r="A83" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
-      <c r="G83" s="2" t="s">
-        <v>239</v>
-      </c>
+      <c r="G83" s="2"/>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="s">
-        <v>241</v>
+      <c r="A84" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>202</v>
+        <v>246</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>238</v>
+        <v>93</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>202</v>
+        <v>94</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
-      <c r="G84" s="2" t="s">
-        <v>239</v>
-      </c>
+      <c r="G84" s="2"/>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="s">
-        <v>242</v>
+      <c r="A85" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>202</v>
+        <v>248</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="2" t="s">
-        <v>239</v>
-      </c>
+      <c r="G85" s="2"/>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="s">
-        <v>243</v>
+      <c r="A86" s="2" t="s">
+        <v>249</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>202</v>
+        <v>250</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="87">
+    </row>
+    <row r="87" ht="28.5">
       <c r="A87" s="1" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>238</v>
+        <v>136</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
-      <c r="G87" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="88">
+      <c r="G87" s="2"/>
+    </row>
+    <row r="88" ht="57">
       <c r="A88" s="1" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>238</v>
+        <v>13</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>202</v>
+        <v>14</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
-      <c r="G88" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="89">
+    </row>
+    <row r="89" ht="42.75">
       <c r="A89" s="1" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>202</v>
+        <v>254</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>238</v>
+        <v>93</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>202</v>
+        <v>94</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
-      <c r="G89" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="90">
+    </row>
+    <row r="90" ht="28.5">
       <c r="A90" s="1" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>238</v>
+        <v>132</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>202</v>
+        <v>133</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
-      <c r="G90" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="91">
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" ht="28.5">
       <c r="A91" s="1" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>202</v>
+        <v>257</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>202</v>
+        <v>259</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="92">
+    </row>
+    <row r="92" ht="71.25">
       <c r="A92" s="1" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>202</v>
+        <v>261</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>238</v>
+        <v>119</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
-      <c r="G103" s="5" t="s">
-        <v>263</v>
+      <c r="G103" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="106" ht="14.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="106">
       <c r="A106" s="1" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>202</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
       <c r="G106" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="107" ht="14.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="107">
       <c r="A107" s="1" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="108" ht="14.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="108">
       <c r="A108" s="1" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="109" ht="14.25">
-      <c r="A109" s="6" t="s">
-        <v>269</v>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="110" ht="14.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="110">
       <c r="A110" s="1" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="111" ht="14.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="111">
       <c r="A111" s="1" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="112" ht="14.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="112">
       <c r="A112" s="1" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="113" ht="14.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="113">
       <c r="A113" s="1" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="114" ht="14.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="114">
       <c r="A114" s="1" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="115" ht="14.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="115">
       <c r="A115" s="1" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="116" ht="14.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="116">
       <c r="A116" s="1" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="1" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
+        <v>165</v>
+      </c>
       <c r="G117" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="1" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="1" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="1" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="1" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="1" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="123" ht="14.25">
       <c r="A123" s="1" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="124" ht="14.25">
       <c r="A124" s="1" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="125" ht="14.25">
       <c r="A125" s="1" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="126" ht="14.25">
       <c r="A126" s="1" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="127" ht="14.25">
       <c r="A127" s="1" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="128" ht="14.25">
       <c r="A128" s="1" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="129" ht="14.25">
       <c r="A129" s="1" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="130" ht="14.25">
       <c r="A130" s="1" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="131" ht="14.25">
       <c r="A131" s="1" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="132" ht="14.25">
       <c r="A132" s="1" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="133" ht="14.25">
       <c r="A133" s="1" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="134" ht="14.25">
       <c r="A134" s="1" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="135" ht="14.25">
       <c r="A135" s="1" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="136" ht="14.25">
       <c r="A136" s="1" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="137" ht="14.25">
       <c r="A137" s="1" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="138" ht="14.25">
       <c r="A138" s="1" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="139" ht="14.25">
       <c r="A139" s="1" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="140" ht="14.25">
       <c r="A140" s="1" t="s">
-        <v>300</v>
+        <v>316</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="141" ht="14.25">
-      <c r="A141" s="1"/>
+      <c r="A141" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="142" ht="14.25">
-      <c r="A142" s="1"/>
+      <c r="A142" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="143" ht="14.25">
-      <c r="A143" s="1"/>
+      <c r="A143" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="144" ht="14.25">
-      <c r="A144" s="1"/>
+      <c r="A144" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="145" ht="14.25">
-      <c r="A145" s="1"/>
+      <c r="A145" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="146" ht="14.25">
-      <c r="A146" s="1"/>
+      <c r="A146" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="147" ht="14.25">
-      <c r="A147" s="1"/>
+      <c r="A147" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="148" ht="14.25">
-      <c r="A148" s="1"/>
+      <c r="A148" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="149" ht="14.25">
-      <c r="A149" s="1"/>
+      <c r="A149" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="150" ht="14.25">
-      <c r="A150" s="1"/>
+      <c r="A150" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="151" ht="14.25">
-      <c r="A151" s="1"/>
+      <c r="A151" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="152" ht="14.25">
       <c r="A152" s="1"/>
@@ -4186,6 +4450,39 @@
     </row>
     <row r="182" ht="14.25">
       <c r="A182" s="1"/>
+    </row>
+    <row r="183" ht="14.25">
+      <c r="A183" s="1"/>
+    </row>
+    <row r="184" ht="14.25">
+      <c r="A184" s="1"/>
+    </row>
+    <row r="185" ht="14.25">
+      <c r="A185" s="1"/>
+    </row>
+    <row r="186" ht="14.25">
+      <c r="A186" s="1"/>
+    </row>
+    <row r="187" ht="14.25">
+      <c r="A187" s="1"/>
+    </row>
+    <row r="188" ht="14.25">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="189" ht="14.25">
+      <c r="A189" s="1"/>
+    </row>
+    <row r="190" ht="14.25">
+      <c r="A190" s="1"/>
+    </row>
+    <row r="191" ht="14.25">
+      <c r="A191" s="1"/>
+    </row>
+    <row r="192" ht="14.25">
+      <c r="A192" s="1"/>
+    </row>
+    <row r="193" ht="14.25">
+      <c r="A193" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Updated documentation downloading script to get some documentation from newer years I was not previously getting. Finished 2019. Began working on 2020.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="380">
   <si>
     <t>variable</t>
   </si>
@@ -122,7 +122,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013, they no longer list the data source as BRFSS, but they start again in 2014. In 2015, they list the source as the CDC Diabetes Interactive Atlas. From 2016-2018, some documentation lists the BRFSS while other documentation lists the CDC Diabetes Interactive Atlas.</t>
+      <t xml:space="preserve">changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013, they no longer list the data source as BRFSS, but they start again in 2014. In 2015, they list the source as the CDC Diabetes Interactive Atlas. From 2016-2019, some documentation lists the BRFSS while other documentation lists the CDC Diabetes Interactive Atlas.</t>
     </r>
   </si>
   <si>
@@ -144,7 +144,7 @@
     <t xml:space="preserve">Percentage of adults ages 20 and older reporting no leisure time physical activity.</t>
   </si>
   <si>
-    <t xml:space="preserve">Starting in 2012, the listed source changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013,  they no longer list the data source as BRFSS, but they start again in 2014. Starting in 2015, they list the source as the CDC DIabetes Interactive Atlas.</t>
+    <t xml:space="preserve">Starting in 2012, the listed source changed to the BRFSS. It is possible this value was always calculated from the BRFSS. In 2013,  they no longer list the data source as BRFSS, but they start again in 2014. Starting in 2015, they list the source as the CDC DIabetes Interactive Atlas. Starting in 2020, they list the source as the US Diabetes Surveillance System.</t>
   </si>
   <si>
     <t>access_to_exercise_opportunities</t>
@@ -225,7 +225,7 @@
     <t xml:space="preserve">National Center for Hepatitis, HIV, STD, and TB Prevention; CDC</t>
   </si>
   <si>
-    <t xml:space="preserve">Numerator and denominator are from different years in the 2010 release.</t>
+    <t xml:space="preserve">Numerator and denominator are from different years in the 2010 release. In the 2010 release, this variable was called chlamydia_rate, but I changed to sexually_transmitted_infections for consistency purposes.</t>
   </si>
   <si>
     <t>teen_births</t>
@@ -264,25 +264,25 @@
     <t>primary_care_physicians</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of primary care providers in patient care per person. The ratio value is the number of people per primary care provider in patient care (reciprocal). Numerator is the number of primary care providers in patient care. The denominator is the number of people.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2018. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+    <t xml:space="preserve">Number of primary care providers in patient care per person. The ratio value is the number of people per primary care provider in patient care (reciprocal). Numerator is the number of primary care providers in patient care. The denominator is the number of people. It should be noted that the documentation states it is the number of doctors per 100,000 people, but it is actually the number of doctors per 1 person.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2019. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
   </si>
   <si>
     <t>dentists</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of dentists per person. The ratio value is the number of people per dentist (reciprocal). Numerator is the number of dentists. Denominator is the number of people.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_dentists to this variable and changed the stem value to ratio from 2012-2018. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+    <t xml:space="preserve">Number of dentists per person. The ratio value is the number of people per dentist (reciprocal). Numerator is the number of dentists. Denominator is the number of people. It should be noted that the documentation states it is the number of doctors per 100,000 people, but it is actually the number of doctors per 1 person.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_dentists to this variable and changed the stem value to ratio from 2012-2019. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
   </si>
   <si>
     <t>mental_health_providers</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of mental health providers per person. The ratio value is the number of people per mental health provider (reciprocal). Numerator is the number of mental health providers. Denominator is the number of people.</t>
+    <t xml:space="preserve">Number of mental health providers per person. The ratio value is the number of people per mental health provider (reciprocal). Numerator is the number of mental health providers. Denominator is the number of people. It should be noted that the documentation states it is the number of doctors per 100,000 people, but it is actually the number of doctors per 1 person.</t>
   </si>
   <si>
     <t xml:space="preserve">cms npi</t>
@@ -291,7 +291,7 @@
     <t xml:space="preserve">CMS National Provider Identification</t>
   </si>
   <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2018. Starting in 2014, the source of the variable changes to cms npi. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2019. Starting in 2014, the source of the variable changes to cms npi. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
   </si>
   <si>
     <t>preventable_hospital_stays</t>
@@ -306,6 +306,15 @@
     <t xml:space="preserve">Medicare claims &amp; Dartmouth Atlas of Health Care</t>
   </si>
   <si>
+    <t>mmdt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mapping Medicare Disparities Tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2019, the source changed to mmdt, and it changed to per 100,000 Medicare enrollees. From 2019-2019, I change the estimate back to per 1000 to make results comparable.</t>
+  </si>
+  <si>
     <t>diabetes_monitoring</t>
   </si>
   <si>
@@ -318,6 +327,15 @@
     <t xml:space="preserve">Percent female Medicare enrollees (age 67-69) having at least 1 mammogram in 2 yrs.</t>
   </si>
   <si>
+    <t xml:space="preserve">In 2019, the source changed to mmdt.</t>
+  </si>
+  <si>
+    <t>flu_vaccinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of annual Medicare enrollees having an annual flu vaccination.</t>
+  </si>
+  <si>
     <t>hospice_use</t>
   </si>
   <si>
@@ -339,7 +357,7 @@
     <t>edfacts</t>
   </si>
   <si>
-    <t xml:space="preserve">State data sources used for Kentucky, New Hampshire, North Carolina, Pennsylvania, South Carolina, and Utah for the years 2010 and 2011. State data sources used for Alaska, Alabama, Arkansas, California, Connecticut, Florida, Hawaii, Idaho, Kentucky, Montana, North Dakota, New Jersey, Oklahoma, South Dakota, and Tennessee in 2012. Unclear in 2013 which states use which data source. Starting in 2014, they mention NCES data is used to supplement data from data.gov. Starting in 2016, the listed source is EDFacts.</t>
+    <t xml:space="preserve">State data sources used for Kentucky, New Hampshire, North Carolina, Pennsylvania, South Carolina, and Utah for the years 2010 and 2011. State data sources used for Alaska, Alabama, Arkansas, California, Connecticut, Florida, Hawaii, Idaho, Kentucky, Montana, North Dakota, New Jersey, Oklahoma, South Dakota, and Tennessee in 2012. Unclear in 2013 which states use which data source. Starting in 2014, they mention NCES data is used to supplement data from data.gov. Starting in 2016, the listed source is EDFacts. Starting in 2019, the listed source is EDFacts and state sources.</t>
   </si>
   <si>
     <t>college_degrees</t>
@@ -513,7 +531,7 @@
     <t xml:space="preserve">At the county level, binary value indicating whether or not the county was exposed to a drinking water violations. 1 = Yes, 0 = No.</t>
   </si>
   <si>
-    <t xml:space="preserve">I rename this variable for the years 2016-2017 to differentiate it from previous years' measure of drinking_water_violations because previous years measured this variable differently. </t>
+    <t xml:space="preserve">I rename this variable for the years 2016-2019 to differentiate it from previous years' measure of drinking_water_violations because previous years measured this variable differently. </t>
   </si>
   <si>
     <t>severe_housing_problems</t>
@@ -528,6 +546,21 @@
     <t xml:space="preserve">Comprehensive Housing Affordability Strategy</t>
   </si>
   <si>
+    <t>percentage_of_households_with_high_housing_costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No documentation available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 2019-2019, I recode the stem value to be raw_value.</t>
+  </si>
+  <si>
+    <t>percentage_of_households_with_overcrowding</t>
+  </si>
+  <si>
+    <t>percentage_of_households_with_lack_of_kitchen_or_plumbing</t>
+  </si>
+  <si>
     <t>driving_alone_to_work</t>
   </si>
   <si>
@@ -567,10 +600,19 @@
     <t xml:space="preserve">Percent of restaurants that are fast food restaurants. Numerator is the number of fast food restaurants, and the denominator is the number of restaurants.</t>
   </si>
   <si>
+    <t>life_expectancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average number of years a person can expect to live.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">national center for health statistics</t>
+  </si>
+  <si>
     <t>premature_age-adjusted_mortality</t>
   </si>
   <si>
-    <t xml:space="preserve">No documentation available.</t>
+    <t xml:space="preserve">Number of deaths under age 75 per 100,000 population (age-adjusted). Numerator is presumably the number of deaths before age 75.</t>
   </si>
   <si>
     <t xml:space="preserve">CDC Wonder and Mortality Data</t>
@@ -579,9 +621,15 @@
     <t>child_mortality</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of deaths among children (under age 18) per 100,000 population.</t>
+  </si>
+  <si>
     <t>infant_mortality</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of infant deaths (within 1 year) per 1000 live births.</t>
+  </si>
+  <si>
     <t>hiw</t>
   </si>
   <si>
@@ -594,9 +642,15 @@
     <t>frequent_physical_distress</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of adults reporting 14 or more days of poor physical health in the past month.</t>
+  </si>
+  <si>
     <t>frequent_mental_distress</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of adults reporting 14 or more days of poor mental health in the past month.</t>
+  </si>
+  <si>
     <t>diabetes_prevalence</t>
   </si>
   <si>
@@ -621,7 +675,7 @@
     <t>hiv_prevalence</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of positive screened individuals for HIV per 100,000 people. Denominator is the total population.</t>
+    <t xml:space="preserve">Number of positive screened individuals for HIV per 100,000 people. In 2020, the listed definition changed to the number of people ages 13 and older living with a HIV diagnosis per 100,000 people.</t>
   </si>
   <si>
     <t xml:space="preserve">hiv nss</t>
@@ -636,6 +690,9 @@
     <t>food_insecurity</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of population who lack adequate access to food.</t>
+  </si>
+  <si>
     <t>mmg</t>
   </si>
   <si>
@@ -645,18 +702,18 @@
     <t>limited_access_to_healthy_foods</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent of people with limited access to health foods. Numerator is the total number of people with limited access to health foods.</t>
+    <t xml:space="preserve">You are definied as having limited access to health foods if you live in poverty and are more than 1 or 10 miles from a grocery store (?). From the documentation, seems a bit confusing.</t>
   </si>
   <si>
     <t xml:space="preserve">USDA Food Environmental Atlas</t>
   </si>
   <si>
-    <t xml:space="preserve">You are definied as having limited access to health foods if you live in poverty and are more than 1 or 10 miles from a grocery store (?). From the documentation, seems a bit confusing.</t>
-  </si>
-  <si>
     <t>drug_overdose_deaths</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of drug poisoning deaths per 100,000 population. Unclear how different this is from the drug_poisoning_deaths variable.</t>
+  </si>
+  <si>
     <t>drug_overdose_deaths_-_modeled</t>
   </si>
   <si>
@@ -666,7 +723,7 @@
     <t>motor_vehicle_crash_deaths</t>
   </si>
   <si>
-    <t xml:space="preserve">Crude motor-vehicle related mortality rate per 100,000 population. Numerator is the total number of motor vehicle-related deaths.</t>
+    <t xml:space="preserve">Crude motor-vehicle related mortality rate per 100,000 population. In 2020, the listed definition changes (?) to the number of motor vehicle crash deaths per 100,000 population.</t>
   </si>
   <si>
     <t xml:space="preserve">national center for health statistics, vital statistics, CDC Wonder and Mortality Data</t>
@@ -675,6 +732,9 @@
     <t>insufficient_sleep</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of adults who report fewer than 7 hours of sleep on average.</t>
+  </si>
+  <si>
     <t>uninsured_adults</t>
   </si>
   <si>
@@ -684,6 +744,9 @@
     <t>uninsured_children</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of children (under 19) without health insurance.</t>
+  </si>
+  <si>
     <t>health_care_costs</t>
   </si>
   <si>
@@ -696,18 +759,45 @@
     <t>other_primary_care_providers</t>
   </si>
   <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers_other_than_physicians to this variable and changed the stem value to ratio for years 2014-2018. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+    <t xml:space="preserve">Number of primary care providers other than physicians per person. The ratio value is the number of people per primary care provider other than physicians (reciprocal). It should be noted that the documentation states it is the number of doctors per 100,000 people, but it is actually the number of doctors per 1 person.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers_other_than_physicians to this variable and changed the stem value to ratio for years 2014-2019. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
   </si>
   <si>
     <t>disconnected_youth</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of people ages 16-19 who are neither working nor in school.</t>
+  </si>
+  <si>
     <t>moa</t>
   </si>
   <si>
     <t xml:space="preserve">measure of america</t>
   </si>
   <si>
+    <t xml:space="preserve">In 2019, the source changes to the acs.</t>
+  </si>
+  <si>
+    <t>reading_scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average grade level performance for 3rd graders on English Language Arts standardized tests.</t>
+  </si>
+  <si>
+    <t>seda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stanford data education archive</t>
+  </si>
+  <si>
+    <t>math_scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average grade level performance for 3rd graders on math standardized tests.</t>
+  </si>
+  <si>
     <t>median_household_income</t>
   </si>
   <si>
@@ -717,7 +807,7 @@
     <t>children_eligible_for_free_lunch</t>
   </si>
   <si>
-    <t xml:space="preserve">Percentage of  children in public schools eligible for free lunch.</t>
+    <t xml:space="preserve">Percentage of children in public schools eligible for free lunch.</t>
   </si>
   <si>
     <t>nces</t>
@@ -729,31 +819,88 @@
     <t>children_eligible_for_free_or_reduced_price_lunch</t>
   </si>
   <si>
+    <t xml:space="preserve">Percentage of children enrolled in public schools that are eligible for free or reduced price lunch.</t>
+  </si>
+  <si>
     <t xml:space="preserve">From 2011-2016, this variable was called children_eligible_for_free_lunch. In 2017, it changed to children_eligible_for_free_or_reduced_price_lunch. It is unclear how, if at all, the variable changed though. The only indication we have of a change in the variable measurment is in 2013, the listed data source changed to the national center for education statistics.</t>
   </si>
   <si>
     <t>residential_segregation_-_black/white</t>
   </si>
   <si>
+    <t xml:space="preserve">Index of dissimilarity where higher values indicate greater residential segregation between Black and White county residents.</t>
+  </si>
+  <si>
     <t>residential_segregation_-_non-white/white</t>
   </si>
   <si>
+    <t xml:space="preserve">Index of dissimilarity where higher values indicate greater residential segregation between non-White and White county residents.</t>
+  </si>
+  <si>
     <t>homicides</t>
   </si>
   <si>
-    <t xml:space="preserve">Age-adjusted homicide rate per 100,000.</t>
+    <t xml:space="preserve">Age-adjusted homicide rate per 100,000. In 2020, the listed definition changes(?) to the number of homicides per 100,000 population.</t>
   </si>
   <si>
     <t xml:space="preserve">In 2016, the source changed to CDC Wonder mortality data. It is unclear if this represents a real change in the data source.</t>
   </si>
   <si>
+    <t>suicides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of suicides per 100,000 population.</t>
+  </si>
+  <si>
     <t>firearm_fatalities</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of deaths due to firearms per 100,000 population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2020, the source changes to nchs. It is unclear if this represents a real change in the variable.</t>
+  </si>
+  <si>
+    <t>juvenile_arrests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate of deliquency cases per 1,000 juveniles.</t>
+  </si>
+  <si>
+    <t>eascjccc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">easy access to state and county juvenile court case counts</t>
+  </si>
+  <si>
+    <t>traffic_volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average traffic volume per meter of major roadways in the county.</t>
+  </si>
+  <si>
+    <t>ejscreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">environmental justice screening and mapping tool</t>
+  </si>
+  <si>
+    <t>homeownership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of occupied housing units that are owned.</t>
+  </si>
+  <si>
+    <t>severe_housing_cost_burden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of households that spent at least 50% of their household income on housing</t>
+  </si>
+  <si>
     <t>population</t>
   </si>
   <si>
-    <t xml:space="preserve">Total population.</t>
+    <t xml:space="preserve">Total resident population.</t>
   </si>
   <si>
     <t>pep</t>
@@ -1057,6 +1204,9 @@
   </si>
   <si>
     <t>colon_cancer_screening</t>
+  </si>
+  <si>
+    <t>opioid_hospital_visits</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1248,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1114,6 +1264,9 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1593,8 +1746,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" style="1" width="46.421875"/>
-    <col customWidth="1" min="2" max="2" style="2" width="80.00390625"/>
+    <col bestFit="1" min="1" max="1" style="1" width="55.7109375"/>
+    <col customWidth="1" min="2" max="2" style="2" width="85.421875"/>
     <col bestFit="1" min="3" max="3" style="1" width="13.33203125"/>
     <col customWidth="1" min="4" max="4" style="2" width="37.57421875"/>
     <col bestFit="1" customWidth="1" min="5" max="5" style="2" width="7.76171875"/>
@@ -1642,7 +1795,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="5"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" ht="28.5">
       <c r="A3" s="1" t="s">
@@ -1708,7 +1861,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" ht="28.5">
       <c r="A7" s="1" t="s">
@@ -1766,7 +1919,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" ht="57">
+    <row r="10" ht="71.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1859,7 +2012,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" ht="28.5">
+    <row r="15" ht="42.75">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -1925,7 +2078,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1933,7 +2086,7 @@
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1952,7 +2105,7 @@
       <c r="A20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1971,7 +2124,7 @@
       <c r="A21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2003,15 +2156,22 @@
       <c r="D22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="23" ht="28.5">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>77</v>
@@ -2022,12 +2182,12 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" ht="28.5">
+    <row r="24" ht="42.75">
       <c r="A24" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>77</v>
@@ -2035,50 +2195,50 @@
       <c r="D24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="25" ht="28.5">
       <c r="A25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" ht="114">
+    </row>
+    <row r="26" ht="28.5">
       <c r="A26" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" ht="28.5">
+        <v>78</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" ht="114">
       <c r="A27" s="1" t="s">
         <v>91</v>
       </c>
@@ -2091,32 +2251,38 @@
       <c r="D27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" ht="42.75">
+      <c r="E27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" ht="28.5">
       <c r="A28" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
     </row>
     <row r="29" ht="42.75">
       <c r="A29" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>99</v>
@@ -2126,205 +2292,199 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-    </row>
-    <row r="30" ht="28.5">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" ht="42.75">
       <c r="A30" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" ht="42.75">
+    <row r="31" ht="28.5">
       <c r="A31" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" ht="28.5">
+    </row>
+    <row r="32" ht="42.75">
       <c r="A32" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="33" ht="28.5">
       <c r="A33" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" ht="28.5">
       <c r="A34" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" ht="99.75">
+    </row>
+    <row r="35" ht="28.5">
       <c r="A35" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" ht="28.5">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" ht="99.75">
       <c r="A36" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="37" ht="28.5">
       <c r="A37" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2" t="s">
-        <v>125</v>
-      </c>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" ht="28.5">
       <c r="A38" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="2" t="s">
         <v>128</v>
       </c>
+      <c r="C38" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="D38" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="39" ht="28.5">
       <c r="A39" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" ht="57">
+    <row r="40" ht="28.5">
       <c r="A40" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="G40" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="41" ht="28.5">
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" ht="57">
       <c r="A41" s="1" t="s">
         <v>140</v>
       </c>
@@ -2332,135 +2492,146 @@
         <v>141</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" ht="42.75">
+        <v>143</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" ht="28.5">
       <c r="A42" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
     <row r="43" ht="42.75">
       <c r="A43" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="44" ht="28.5">
+    </row>
+    <row r="44" ht="42.75">
       <c r="A44" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-    </row>
-    <row r="45" ht="42.75">
+      <c r="G44" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" ht="28.5">
       <c r="A45" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
     </row>
     <row r="46" ht="28.5">
       <c r="A46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>160</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="G46" s="5" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="47" ht="28.5">
       <c r="A47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="5" t="s">
+      <c r="G47" s="2" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="48" ht="28.5">
       <c r="A48" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-    </row>
-    <row r="49" ht="28.5">
+      <c r="G48" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" ht="42.75">
       <c r="A49" s="1" t="s">
         <v>164</v>
       </c>
@@ -2468,13 +2639,14 @@
         <v>165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
     </row>
     <row r="50" ht="28.5">
       <c r="A50" s="1" t="s">
@@ -2484,10 +2656,10 @@
         <v>167</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>168</v>
+        <v>100</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -2495,318 +2667,307 @@
     </row>
     <row r="51" ht="28.5">
       <c r="A51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" ht="42.75">
+      <c r="G51" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" ht="28.5">
       <c r="A52" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>173</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" ht="28.5">
       <c r="A53" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
     </row>
     <row r="54" ht="28.5">
       <c r="A54" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>14</v>
+        <v>177</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" ht="57">
+    </row>
+    <row r="55" ht="28.5">
       <c r="A55" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G55" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="56" ht="42.75">
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" ht="28.5">
       <c r="A56" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="5" t="s">
         <v>184</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>50</v>
+        <v>142</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" ht="42.75">
+      <c r="A57" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="B57" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="C57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="57" ht="28.5">
-      <c r="A57" s="1" t="s">
+      <c r="F57" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="G57" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D57" s="2" t="s">
+    </row>
+    <row r="58" ht="28.5">
+      <c r="A58" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" ht="42.75">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="C58" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>193</v>
+        <v>14</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="2" t="s">
-        <v>194</v>
-      </c>
+      <c r="G58" s="2"/>
     </row>
     <row r="59" ht="28.5">
       <c r="A59" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>167</v>
+        <v>192</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>168</v>
+        <v>14</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" ht="114">
+    <row r="60" ht="57">
       <c r="A60" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="I60" s="1"/>
-    </row>
-    <row r="61" ht="28.5">
+      <c r="E60" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" ht="42.75">
       <c r="A61" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>128</v>
+        <v>201</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="62" ht="28.5">
       <c r="A62" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>167</v>
+        <v>206</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>13</v>
+        <v>208</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>14</v>
+        <v>209</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" ht="28.5">
+    <row r="63" ht="42.75">
       <c r="A63" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>58</v>
+        <v>212</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
     <row r="64" ht="28.5">
       <c r="A64" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>167</v>
+        <v>213</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>214</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>58</v>
+        <v>182</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" ht="28.5">
+    <row r="65" ht="114">
       <c r="A65" s="1" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>206</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
       <c r="G65" s="2" t="s">
-        <v>207</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="I65" s="1"/>
     </row>
     <row r="66" ht="28.5">
       <c r="A66" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>72</v>
+        <v>217</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>73</v>
+        <v>219</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="5" t="s">
-        <v>209</v>
-      </c>
+      <c r="G66" s="2"/>
     </row>
     <row r="67" ht="28.5">
       <c r="A67" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>167</v>
+        <v>220</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>212</v>
+        <v>14</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -2814,16 +2975,16 @@
     </row>
     <row r="68" ht="28.5">
       <c r="A68" s="1" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -2831,1581 +2992,1785 @@
     </row>
     <row r="69" ht="28.5">
       <c r="A69" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>216</v>
+        <v>224</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>225</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>218</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
     </row>
     <row r="70" ht="28.5">
       <c r="A70" s="1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>217</v>
+        <v>61</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="G70" s="2" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
     </row>
     <row r="71" ht="28.5">
       <c r="A71" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>167</v>
+        <v>229</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
+      <c r="G71" s="5" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="72" ht="28.5">
       <c r="A72" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>167</v>
+        <v>232</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>233</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>93</v>
+        <v>234</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
+        <v>235</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="73" ht="28.5">
       <c r="A73" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>225</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
     </row>
     <row r="74" ht="28.5">
       <c r="A74" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>228</v>
+        <v>241</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+    </row>
+    <row r="75" ht="28.5">
+      <c r="A75" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>244</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>229</v>
+        <v>109</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>232</v>
+    <row r="76" ht="28.5">
+      <c r="A76" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>229</v>
+        <v>30</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>234</v>
+        <v>212</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="77" ht="28.5">
+      <c r="A77" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>230</v>
+        <v>94</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>236</v>
+      <c r="G77" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="78" ht="28.5">
+      <c r="A78" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>229</v>
+        <v>99</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>230</v>
+        <v>100</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>238</v>
+    <row r="79" ht="28.5">
+      <c r="A79" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>229</v>
+        <v>99</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>230</v>
+        <v>100</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
     </row>
-    <row r="80">
-      <c r="A80" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>240</v>
+    <row r="80" ht="28.5">
+      <c r="A80" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>229</v>
+        <v>9</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="81" ht="28.5">
-      <c r="A81" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>230</v>
+      <c r="A81" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
     </row>
-    <row r="82">
-      <c r="A82" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>244</v>
+    <row r="82" ht="28.5">
+      <c r="A82" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>229</v>
+        <v>142</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>230</v>
+        <v>182</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="83" ht="28.5">
+      <c r="A83" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+    </row>
+    <row r="84" ht="28.5">
+      <c r="A84" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+    </row>
+    <row r="85" ht="28.5">
+      <c r="A85" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
     </row>
-    <row r="86">
-      <c r="A86" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>230</v>
+    <row r="86" ht="28.5">
+      <c r="A86" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
-    </row>
-    <row r="87" ht="28.5">
-      <c r="A87" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>167</v>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>277</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>136</v>
+        <v>278</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" ht="57">
-      <c r="A88" s="1" t="s">
-        <v>254</v>
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>167</v>
+        <v>281</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>13</v>
+        <v>278</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>14</v>
+        <v>279</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
-    </row>
-    <row r="89" ht="42.75">
-      <c r="A89" s="1" t="s">
-        <v>255</v>
+      <c r="G88" s="2"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="s">
+        <v>282</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>93</v>
+        <v>278</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>94</v>
+        <v>279</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
-    </row>
-    <row r="90" ht="28.5">
-      <c r="A90" s="1" t="s">
-        <v>257</v>
+      <c r="G89" s="2"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="s">
+        <v>284</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>167</v>
+        <v>285</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>132</v>
+        <v>278</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>133</v>
+        <v>279</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" ht="28.5">
-      <c r="A91" s="1" t="s">
-        <v>258</v>
+    <row r="91">
+      <c r="A91" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-    </row>
-    <row r="92" ht="71.25">
-      <c r="A92" s="1" t="s">
-        <v>262</v>
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>119</v>
+        <v>278</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
-      <c r="G92" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="s">
-        <v>266</v>
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" ht="28.5">
+      <c r="A93" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>167</v>
+        <v>291</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>167</v>
+        <v>279</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
-      <c r="G93" s="2" t="s">
-        <v>268</v>
-      </c>
+      <c r="G93" s="2"/>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="s">
-        <v>269</v>
+      <c r="A94" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>167</v>
+        <v>293</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>167</v>
+        <v>279</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
-      <c r="G94" s="2" t="s">
-        <v>268</v>
-      </c>
+      <c r="G94" s="2"/>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="s">
-        <v>270</v>
+      <c r="A95" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>167</v>
+        <v>295</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>167</v>
+        <v>279</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
-      <c r="G95" s="2" t="s">
-        <v>268</v>
-      </c>
+      <c r="G95" s="2"/>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="s">
-        <v>271</v>
+      <c r="A96" s="2" t="s">
+        <v>296</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>167</v>
+        <v>297</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>267</v>
+        <v>99</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
-      <c r="G96" s="2" t="s">
-        <v>268</v>
-      </c>
+      <c r="G96" s="2"/>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="s">
-        <v>272</v>
+      <c r="A97" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>167</v>
+        <v>299</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>167</v>
+        <v>279</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
-      <c r="G97" s="2" t="s">
-        <v>268</v>
-      </c>
+      <c r="G97" s="2"/>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="s">
-        <v>273</v>
+      <c r="A98" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>167</v>
+        <v>301</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>167</v>
+        <v>279</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
-      <c r="G98" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="99">
+    </row>
+    <row r="99" ht="28.5">
       <c r="A99" s="1" t="s">
-        <v>274</v>
+        <v>302</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>267</v>
+        <v>142</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
-      <c r="G99" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="100">
+      <c r="G99" s="2"/>
+    </row>
+    <row r="100" ht="57">
       <c r="A100" s="1" t="s">
-        <v>275</v>
+        <v>303</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>267</v>
+        <v>13</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>167</v>
+        <v>14</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
-      <c r="G100" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="101">
+    </row>
+    <row r="101" ht="42.75">
       <c r="A101" s="1" t="s">
-        <v>276</v>
+        <v>304</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>167</v>
+        <v>305</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>267</v>
+        <v>99</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
-      <c r="G101" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="102">
+    </row>
+    <row r="102" ht="28.5">
       <c r="A102" s="1" t="s">
-        <v>278</v>
+        <v>306</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>267</v>
+        <v>138</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
-      <c r="G102" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="103">
+      <c r="G102" s="2"/>
+    </row>
+    <row r="103" ht="28.5">
       <c r="A103" s="1" t="s">
-        <v>279</v>
+        <v>307</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>167</v>
+        <v>308</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>167</v>
+        <v>310</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
-      <c r="G103" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="104">
+    </row>
+    <row r="104" ht="71.25">
       <c r="A104" s="1" t="s">
-        <v>280</v>
+        <v>311</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>167</v>
+        <v>312</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>267</v>
+        <v>125</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>167</v>
+        <v>313</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2" t="s">
-        <v>277</v>
+        <v>314</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>281</v>
+        <v>315</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2" t="s">
-        <v>277</v>
+        <v>317</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>282</v>
+        <v>318</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2" t="s">
-        <v>277</v>
+        <v>317</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>283</v>
+        <v>319</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2" t="s">
-        <v>277</v>
+        <v>317</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>284</v>
+        <v>320</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2" t="s">
-        <v>285</v>
+        <v>317</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>286</v>
+        <v>321</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2" t="s">
-        <v>285</v>
+        <v>317</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="s">
-        <v>287</v>
+        <v>322</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2" t="s">
-        <v>285</v>
+        <v>317</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
-        <v>288</v>
+        <v>323</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2" t="s">
-        <v>285</v>
+        <v>317</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="s">
-        <v>289</v>
+        <v>324</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2" t="s">
-        <v>285</v>
+        <v>317</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2" t="s">
-        <v>285</v>
+        <v>326</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
-        <v>291</v>
+        <v>327</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2" t="s">
-        <v>292</v>
+        <v>326</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
-        <v>293</v>
+        <v>328</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2" t="s">
-        <v>285</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
-        <v>294</v>
+        <v>329</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="117" ht="14.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="117">
       <c r="A117" s="1" t="s">
-        <v>295</v>
+        <v>330</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>167</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
       <c r="G117" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="118" ht="14.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="118">
       <c r="A118" s="1" t="s">
-        <v>296</v>
+        <v>331</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="119" ht="14.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="119">
       <c r="A119" s="1" t="s">
-        <v>297</v>
+        <v>332</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="120" ht="14.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="120">
       <c r="A120" s="1" t="s">
-        <v>298</v>
+        <v>333</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="121" ht="14.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="121">
       <c r="A121" s="1" t="s">
-        <v>299</v>
+        <v>335</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="122" ht="14.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="122">
       <c r="A122" s="1" t="s">
-        <v>300</v>
+        <v>336</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="123" ht="14.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="123">
       <c r="A123" s="1" t="s">
-        <v>301</v>
+        <v>337</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="124" ht="14.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="124">
       <c r="A124" s="1" t="s">
-        <v>302</v>
+        <v>338</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="125" ht="14.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="125">
       <c r="A125" s="1" t="s">
-        <v>303</v>
+        <v>339</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="126" ht="14.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="126">
       <c r="A126" s="1" t="s">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="127" ht="14.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="127">
       <c r="A127" s="1" t="s">
-        <v>305</v>
+        <v>342</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="128" ht="14.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="128">
       <c r="A128" s="1" t="s">
-        <v>306</v>
+        <v>343</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="129" ht="14.25">
       <c r="A129" s="1" t="s">
-        <v>307</v>
+        <v>344</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E129" s="2"/>
-      <c r="F129" s="2"/>
+        <v>160</v>
+      </c>
       <c r="G129" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="130" ht="14.25">
       <c r="A130" s="1" t="s">
-        <v>308</v>
+        <v>345</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="131" ht="14.25">
       <c r="A131" s="1" t="s">
-        <v>309</v>
+        <v>346</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="132" ht="14.25">
       <c r="A132" s="1" t="s">
-        <v>310</v>
+        <v>347</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="133" ht="14.25">
       <c r="A133" s="1" t="s">
-        <v>311</v>
+        <v>348</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="134" ht="14.25">
       <c r="A134" s="1" t="s">
-        <v>312</v>
+        <v>349</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="135" ht="14.25">
       <c r="A135" s="1" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="136" ht="14.25">
       <c r="A136" s="1" t="s">
-        <v>314</v>
+        <v>351</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="137" ht="14.25">
       <c r="A137" s="1" t="s">
-        <v>315</v>
+        <v>352</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="138" ht="14.25">
       <c r="A138" s="1" t="s">
-        <v>316</v>
+        <v>353</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="139" ht="14.25">
       <c r="A139" s="1" t="s">
-        <v>317</v>
+        <v>354</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="140" ht="14.25">
       <c r="A140" s="1" t="s">
-        <v>318</v>
+        <v>355</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="141" ht="14.25">
       <c r="A141" s="1" t="s">
-        <v>319</v>
+        <v>356</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="142" ht="14.25">
       <c r="A142" s="1" t="s">
-        <v>320</v>
+        <v>357</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="143" ht="14.25">
       <c r="A143" s="1" t="s">
-        <v>321</v>
+        <v>358</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="144" ht="14.25">
       <c r="A144" s="1" t="s">
-        <v>322</v>
+        <v>359</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
       <c r="G144" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="145" ht="14.25">
       <c r="A145" s="1" t="s">
-        <v>323</v>
+        <v>360</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="146" ht="14.25">
       <c r="A146" s="1" t="s">
-        <v>324</v>
+        <v>361</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="147" ht="14.25">
       <c r="A147" s="1" t="s">
-        <v>325</v>
+        <v>362</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="148" ht="14.25">
       <c r="A148" s="1" t="s">
-        <v>326</v>
+        <v>363</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="149" ht="14.25">
       <c r="A149" s="1" t="s">
-        <v>327</v>
+        <v>364</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="150" ht="14.25">
       <c r="A150" s="1" t="s">
-        <v>328</v>
+        <v>365</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="151" ht="14.25">
       <c r="A151" s="1" t="s">
-        <v>329</v>
+        <v>366</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
     </row>
     <row r="152" ht="14.25">
-      <c r="A152" s="1"/>
+      <c r="A152" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="153" ht="14.25">
-      <c r="A153" s="1"/>
+      <c r="A153" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="154" ht="14.25">
-      <c r="A154" s="1"/>
+      <c r="A154" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="155" ht="14.25">
-      <c r="A155" s="1"/>
+      <c r="A155" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="156" ht="14.25">
-      <c r="A156" s="1"/>
+      <c r="A156" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="157" ht="14.25">
-      <c r="A157" s="1"/>
+      <c r="A157" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="158" ht="14.25">
-      <c r="A158" s="1"/>
+      <c r="A158" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="159" ht="14.25">
-      <c r="A159" s="1"/>
+      <c r="A159" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="160" ht="14.25">
-      <c r="A160" s="1"/>
+      <c r="A160" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="161" ht="14.25">
-      <c r="A161" s="1"/>
+      <c r="A161" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="162" ht="14.25">
-      <c r="A162" s="1"/>
+      <c r="A162" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="163" ht="14.25">
-      <c r="A163" s="1"/>
+      <c r="A163" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="164" ht="14.25">
-      <c r="A164" s="1"/>
+      <c r="A164" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="165" ht="14.25">
       <c r="A165" s="1"/>
@@ -4493,6 +4858,42 @@
     </row>
     <row r="193" ht="14.25">
       <c r="A193" s="1"/>
+    </row>
+    <row r="194" ht="14.25">
+      <c r="A194" s="1"/>
+    </row>
+    <row r="195" ht="14.25">
+      <c r="A195" s="1"/>
+    </row>
+    <row r="196" ht="14.25">
+      <c r="A196" s="1"/>
+    </row>
+    <row r="197" ht="14.25">
+      <c r="A197" s="1"/>
+    </row>
+    <row r="198" ht="14.25">
+      <c r="A198" s="1"/>
+    </row>
+    <row r="199" ht="14.25">
+      <c r="A199" s="1"/>
+    </row>
+    <row r="200" ht="14.25">
+      <c r="A200" s="1"/>
+    </row>
+    <row r="201" ht="14.25">
+      <c r="A201" s="1"/>
+    </row>
+    <row r="202" ht="14.25">
+      <c r="A202" s="1"/>
+    </row>
+    <row r="203" ht="14.25">
+      <c r="A203" s="1"/>
+    </row>
+    <row r="204" ht="14.25">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205" ht="14.25">
+      <c r="A205" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Began 2021. Made decent progress. Need to fix mammography.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -81,7 +81,7 @@
     <t xml:space="preserve">Percent of births with low birth weight (&lt;2500g). Numerator is the number of births with low birth weight. Denominator is the total number of live births.</t>
   </si>
   <si>
-    <t xml:space="preserve">Starting in 2020, each observation gets marked as unreliable or not. Observations are unreliable if, "... the relative standard error for the estimate is greater than 20% or when the number of LBW births is less than 20." From 2020-2020, I change the flag name from lbw to low_birthweight to match the full variable name.</t>
+    <t xml:space="preserve">Starting in 2020, each observation gets marked as unreliable or not. Observations are unreliable if, "... the relative standard error for the estimate is greater than 20% or when the number of LBW births is less than 20." From 2020-2021, I change the flag name from lbw to low_birthweight to match the full variable name.</t>
   </si>
   <si>
     <t>adult_smoking</t>
@@ -273,7 +273,7 @@
     <t xml:space="preserve">Number of primary care providers in patient care per person. The ratio value is the number of people per primary care provider in patient care (reciprocal). Numerator is the number of primary care providers in patient care. The denominator is the number of people. It should be noted that the documentation states it is the number of doctors per 100,000 people, but it is actually the number of doctors per 1 person.</t>
   </si>
   <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2020. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2021. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
   </si>
   <si>
     <t>dentists</t>
@@ -282,7 +282,7 @@
     <t xml:space="preserve">Number of dentists per person. The ratio value is the number of people per dentist (reciprocal). Numerator is the number of dentists. Denominator is the number of people. It should be noted that the documentation states it is the number of doctors per 100,000 people, but it is actually the number of doctors per 1 person.</t>
   </si>
   <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_dentists to this variable and changed the stem value to ratio from 2012-2020. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+    <t xml:space="preserve">I recode the ratio_of_population_to_dentists to this variable and changed the stem value to ratio from 2012-2021. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
   </si>
   <si>
     <t>mental_health_providers</t>
@@ -297,7 +297,7 @@
     <t xml:space="preserve">CMS National Provider Identification</t>
   </si>
   <si>
-    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2020. Starting in 2014, the source of the variable changes to cms npi. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
+    <t xml:space="preserve">I recode the ratio_of_population_to_primary_care_providers to this variable and changed the stem value to ratio from 2011-2021. Starting in 2014, the source of the variable changes to cms npi. Concerning the ratio variable, "When a county has no reported providers, the value for the ratio variable is assigned to be the negative population value. This means for  counties with zero providers, the value is stored as a negative number (e.g., if the ratio is 2000:0, the value stored in the field would be -2000.)"</t>
   </si>
   <si>
     <t>preventable_hospital_stays</t>
@@ -318,7 +318,7 @@
     <t xml:space="preserve">Mapping Medicare Disparities Tool</t>
   </si>
   <si>
-    <t xml:space="preserve">In 2019, the source changed to mmdt, and it changed to per 100,000 Medicare enrollees. From 2019-2020, I change the estimate back to per 1000 to make results comparable.</t>
+    <t xml:space="preserve">In 2019, the source changed to mmdt, and it changed to per 100,000 Medicare enrollees. From 2019-2021, I change the estimate back to per 1000 to make results comparable.</t>
   </si>
   <si>
     <t>diabetes_monitoring</t>
@@ -1271,17 +1271,17 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1294,9 +1294,6 @@
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1779,8 +1776,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" style="1" width="71.19140625"/>
-    <col customWidth="1" min="2" max="2" style="2" width="85.421875"/>
+    <col customWidth="1" min="1" max="1" style="1" width="37.28125"/>
+    <col customWidth="1" min="2" max="2" style="2" width="60.28125"/>
     <col bestFit="1" min="3" max="3" style="1" width="15.953125"/>
     <col customWidth="1" min="4" max="4" style="2" width="37.57421875"/>
     <col bestFit="1" customWidth="1" min="5" max="5" style="2" width="7.76171875"/>
@@ -1814,7 +1811,7 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" ht="42.75">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1828,7 +1825,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1896,7 +1893,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1916,7 +1913,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" ht="99.75">
+    <row r="8" ht="85.5">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1935,11 +1932,11 @@
       <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" ht="28.5">
+    <row r="9" ht="42.75">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1975,7 +1972,7 @@
       <c r="F10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2068,7 +2065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" ht="28.5">
+    <row r="16" ht="42.75">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -2100,7 +2097,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" ht="199.5">
+    <row r="18" ht="185.25">
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
@@ -2134,7 +2131,7 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2153,7 +2150,7 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2176,7 +2173,7 @@
       <c r="F21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2199,7 +2196,7 @@
       <c r="F22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2223,7 +2220,7 @@
       <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -2238,7 +2235,7 @@
       <c r="F24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="5" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2314,7 +2311,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" ht="28.5">
+    <row r="29" ht="42.75">
       <c r="A29" s="1" t="s">
         <v>103</v>
       </c>
@@ -2331,7 +2328,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" ht="42.75">
+    <row r="30" ht="57">
       <c r="A30" s="1" t="s">
         <v>105</v>
       </c>
@@ -2360,13 +2357,13 @@
       <c r="D31" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="2" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2406,7 +2403,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" ht="28.5">
+    <row r="34" ht="42.75">
       <c r="A34" s="1" t="s">
         <v>119</v>
       </c>
@@ -2475,7 +2472,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" ht="28.5">
+    <row r="38" ht="42.75">
       <c r="A38" s="1" t="s">
         <v>130</v>
       </c>
@@ -2567,7 +2564,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" ht="42.75">
+    <row r="43" ht="57">
       <c r="A43" s="1" t="s">
         <v>151</v>
       </c>
@@ -2598,11 +2595,11 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="6" t="s">
+      <c r="G44" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="45" ht="28.5">
+    <row r="45" ht="42.75">
       <c r="A45" s="1" t="s">
         <v>158</v>
       </c>
@@ -2633,7 +2630,7 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="6" t="s">
+      <c r="G46" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2652,7 +2649,7 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="6" t="s">
+      <c r="G47" s="2" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2671,11 +2668,11 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="6" t="s">
+      <c r="G48" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="49" ht="42.75">
+    <row r="49" ht="57">
       <c r="A49" s="1" t="s">
         <v>167</v>
       </c>
@@ -2692,7 +2689,7 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" ht="28.5">
+    <row r="50" ht="42.75">
       <c r="A50" s="1" t="s">
         <v>169</v>
       </c>
@@ -2709,7 +2706,7 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" ht="28.5">
+    <row r="51" ht="42.75">
       <c r="A51" s="1" t="s">
         <v>171</v>
       </c>
@@ -2728,7 +2725,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" ht="28.5">
+    <row r="52" ht="42.75">
       <c r="A52" s="1" t="s">
         <v>176</v>
       </c>
@@ -2744,7 +2741,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" ht="28.5">
+    <row r="53" ht="42.75">
       <c r="A53" s="1" t="s">
         <v>178</v>
       </c>
@@ -2776,17 +2773,17 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" ht="28.5">
+    <row r="55" ht="42.75">
       <c r="A55" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="2" t="s">
         <v>185</v>
       </c>
       <c r="E55" s="2"/>
@@ -2800,10 +2797,10 @@
       <c r="B56" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="2" t="s">
         <v>188</v>
       </c>
       <c r="E56" s="2"/>
@@ -2817,10 +2814,10 @@
       <c r="B57" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="2" t="s">
         <v>185</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -2829,7 +2826,7 @@
       <c r="F57" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G57" s="2" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2886,7 +2883,7 @@
       <c r="F60" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="G60" s="2" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2930,7 +2927,7 @@
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" ht="28.5">
+    <row r="63" ht="42.75">
       <c r="A63" s="1" t="s">
         <v>214</v>
       </c>
@@ -2953,10 +2950,10 @@
       <c r="B64" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="2" t="s">
         <v>185</v>
       </c>
       <c r="E64" s="2"/>
@@ -3089,7 +3086,7 @@
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="6" t="s">
+      <c r="G71" s="2" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3165,7 +3162,7 @@
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="6" t="s">
+      <c r="G75" s="2" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3252,10 +3249,10 @@
       <c r="B80" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C80" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D80" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E80" s="2"/>
@@ -3280,10 +3277,10 @@
       <c r="G81" s="2"/>
     </row>
     <row r="82" ht="28.5">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C82" s="1" t="s">
@@ -3294,7 +3291,7 @@
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
-      <c r="G82" s="6" t="s">
+      <c r="G82" s="2" t="s">
         <v>266</v>
       </c>
     </row>
@@ -3305,10 +3302,10 @@
       <c r="B83" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D83" s="2" t="s">
         <v>185</v>
       </c>
       <c r="E83" s="2"/>
@@ -3333,10 +3330,10 @@
       <c r="G84" s="2"/>
     </row>
     <row r="85" ht="28.5">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B85" s="2" t="s">
         <v>274</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -3347,7 +3344,7 @@
       </c>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="6" t="s">
+      <c r="G85" s="2" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3355,7 +3352,7 @@
       <c r="A86" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="2" t="s">
         <v>277</v>
       </c>
       <c r="C86" s="1" t="s">

</xml_diff>

<commit_message>
Round 2 of documentation.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="437">
   <si>
     <t>variable</t>
   </si>
@@ -93,7 +93,7 @@
     <t>adult_obesity</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent of adults that report BMI &gt;= 30.</t>
+    <t xml:space="preserve">Percentage of the adult population (ages 18 and older) that reports a body mass index (BMI) greater than or equal to 30 kg/m^2.</t>
   </si>
   <si>
     <t>nccdphp</t>
@@ -192,7 +192,7 @@
     <t xml:space="preserve">OneSource Global Business Browser, Delorme map data, ESRI, &amp; US Census Tigerline Files</t>
   </si>
   <si>
-    <t xml:space="preserve">Starting in 2022, the documentation states  YMCA shapefiles were used while no mention is made off Delorme map data. Starting in 2023, the documentation lists the Living Atlas of the World and not the OneSource Global Business Browser.</t>
+    <t xml:space="preserve">Starting in 2022, the documentation states YMCA shapefiles were used while no mention is made off Delorme map data. Starting in 2023, the documentation lists the Living Atlas of the World and not the OneSource Global Business Browser.</t>
   </si>
   <si>
     <t>binge_drinking</t>
@@ -1086,24 +1086,30 @@
     <t xml:space="preserve">From 2011 to 2019, I rename the variable from %_non-hispanic_african_american to %_non-hispanic_black for consistency purposes as newer releases of the data use Black instead of African-American.</t>
   </si>
   <si>
-    <t>%_american_indian_and_alaskan_native</t>
+    <t>%_american_indian_or_alaska_native</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage of total population that is American Indian or an Alaskan Native.</t>
   </si>
   <si>
+    <t xml:space="preserve">From 2011 to 2019, I rename the variable from %_american_indian_and_alaskan_native to %_american_indian_or_alaska_native AND from 2020 to 2022, I rename %_american_indian_&amp;_alaska_native to %_american_indian_or_alaska_native  for concistency purposes with newer releases of the data. </t>
+  </si>
+  <si>
     <t>%_asian</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage of total population that is Asian.</t>
   </si>
   <si>
-    <t>%_native_hawaiian/other_pacific_islander</t>
+    <t>%_native_hawaiian_or_other_pacific_islander</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage of total population that is Native Hawaiiian or an other Pacific Islander.</t>
   </si>
   <si>
+    <t xml:space="preserve">From 2011-2022, I rename %_native_hawaiian/other_pacific_islander to %_native_hawaiian_or_other_pacific_islander to match the newest release of the data.</t>
+  </si>
+  <si>
     <t>%_hispanic</t>
   </si>
   <si>
@@ -1122,10 +1128,13 @@
     <t xml:space="preserve">Percentage of total population that is not proficient in English.</t>
   </si>
   <si>
-    <t>%_females</t>
+    <t>%_female</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage of total population that is female.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 2011 to 2021, I rename the variable from %_females to %_female for consistency purposes with newer releases of the data.</t>
   </si>
   <si>
     <t>%_rural</t>
@@ -1439,7 +1448,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1461,9 +1470,6 @@
     </xf>
     <xf fontId="3" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1936,14 +1942,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="1" width="37.28125"/>
+    <col customWidth="1" min="1" max="1" style="1" width="41.421875"/>
     <col customWidth="1" min="2" max="2" style="2" width="60.28125"/>
     <col bestFit="1" min="3" max="3" style="1" width="15.953125"/>
     <col customWidth="1" min="4" max="4" style="2" width="37.57421875"/>
@@ -2060,7 +2066,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2084,7 +2090,7 @@
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2143,7 +2149,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" ht="42.75">
+    <row r="11" ht="57">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -2158,7 +2164,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2300,7 +2306,7 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2319,7 +2325,7 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2342,7 +2348,7 @@
       <c r="F21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2365,7 +2371,7 @@
       <c r="F22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="2" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2398,7 +2404,7 @@
       <c r="D24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="2" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2794,7 +2800,7 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="5" t="s">
+      <c r="G46" s="2" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2829,7 +2835,7 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="5" t="s">
+      <c r="G48" s="2" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2848,7 +2854,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="5" t="s">
+      <c r="G49" s="2" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2867,7 +2873,7 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="5" t="s">
+      <c r="G50" s="2" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3231,7 +3237,7 @@
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="5" t="s">
+      <c r="G70" s="2" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3307,7 +3313,7 @@
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="5" t="s">
+      <c r="G74" s="2" t="s">
         <v>245</v>
       </c>
     </row>
@@ -3616,7 +3622,7 @@
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="5" t="s">
+      <c r="G91" s="2" t="s">
         <v>298</v>
       </c>
     </row>
@@ -3669,7 +3675,7 @@
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
-      <c r="G94" s="5" t="s">
+      <c r="G94" s="2" t="s">
         <v>307</v>
       </c>
     </row>
@@ -3688,43 +3694,43 @@
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
-      <c r="G95" s="5" t="s">
+      <c r="G95" s="2" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="96" ht="28.5">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C96" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="2" t="s">
         <v>313</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
-      <c r="G96" s="5"/>
+      <c r="G96" s="2"/>
     </row>
     <row r="97" ht="28.5">
-      <c r="A97" s="8" t="s">
+      <c r="A97" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="2" t="s">
         <v>317</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
-      <c r="G97" s="5"/>
+      <c r="G97" s="2"/>
     </row>
     <row r="98" ht="28.5">
       <c r="A98" s="1" t="s">
@@ -3879,14 +3885,16 @@
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
-      <c r="G106" s="2"/>
+      <c r="G106" s="2" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>330</v>
@@ -3900,10 +3908,10 @@
     </row>
     <row r="108" ht="28.5">
       <c r="A108" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>330</v>
@@ -3913,14 +3921,16 @@
       </c>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
+      <c r="G108" s="2" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>330</v>
@@ -3934,10 +3944,10 @@
     </row>
     <row r="110">
       <c r="A110" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>330</v>
@@ -3951,10 +3961,10 @@
     </row>
     <row r="111">
       <c r="A111" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>105</v>
@@ -3968,10 +3978,10 @@
     </row>
     <row r="112">
       <c r="A112" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>330</v>
@@ -3981,14 +3991,16 @@
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
+      <c r="G112" s="2" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>330</v>
@@ -4001,7 +4013,7 @@
     </row>
     <row r="114" ht="28.5">
       <c r="A114" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>169</v>
@@ -4010,7 +4022,7 @@
         <v>151</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -4018,7 +4030,7 @@
     </row>
     <row r="115" ht="57">
       <c r="A115" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>169</v>
@@ -4034,10 +4046,10 @@
     </row>
     <row r="116" ht="42.75">
       <c r="A116" s="1" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>105</v>
@@ -4050,7 +4062,7 @@
     </row>
     <row r="117" ht="28.5">
       <c r="A117" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>169</v>
@@ -4067,48 +4079,48 @@
     </row>
     <row r="118" ht="28.5">
       <c r="A118" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
     </row>
     <row r="119" ht="71.25">
       <c r="A119" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>169</v>
@@ -4116,18 +4128,18 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>169</v>
@@ -4135,18 +4147,18 @@
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>169</v>
@@ -4154,18 +4166,18 @@
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>169</v>
@@ -4173,18 +4185,18 @@
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>169</v>
@@ -4192,18 +4204,18 @@
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>169</v>
@@ -4211,18 +4223,18 @@
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>169</v>
@@ -4230,18 +4242,18 @@
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>169</v>
@@ -4249,18 +4261,18 @@
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>169</v>
@@ -4268,18 +4280,18 @@
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>169</v>
@@ -4287,18 +4299,18 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>169</v>
@@ -4306,18 +4318,18 @@
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>169</v>
@@ -4325,18 +4337,18 @@
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>169</v>
@@ -4344,18 +4356,18 @@
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>169</v>
@@ -4363,18 +4375,18 @@
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>169</v>
@@ -4382,18 +4394,18 @@
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>169</v>
@@ -4401,18 +4413,18 @@
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>169</v>
@@ -4420,18 +4432,18 @@
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>169</v>
@@ -4439,18 +4451,18 @@
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>169</v>
@@ -4458,18 +4470,18 @@
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>169</v>
@@ -4477,18 +4489,18 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>169</v>
@@ -4496,18 +4508,18 @@
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>169</v>
@@ -4515,18 +4527,18 @@
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>169</v>
@@ -4534,18 +4546,18 @@
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>169</v>
@@ -4553,35 +4565,35 @@
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="144" ht="14.25">
       <c r="A144" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>169</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="145" ht="14.25">
       <c r="A145" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>169</v>
@@ -4589,18 +4601,18 @@
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="146" ht="14.25">
       <c r="A146" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>169</v>
@@ -4608,18 +4620,18 @@
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="147" ht="14.25">
       <c r="A147" s="1" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>169</v>
@@ -4627,18 +4639,18 @@
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="148" ht="14.25">
       <c r="A148" s="1" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>169</v>
@@ -4646,18 +4658,18 @@
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="149" ht="14.25">
       <c r="A149" s="1" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>169</v>
@@ -4665,18 +4677,18 @@
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="150" ht="14.25">
       <c r="A150" s="1" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>169</v>
@@ -4684,18 +4696,18 @@
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="151" ht="14.25">
       <c r="A151" s="1" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>169</v>
@@ -4703,18 +4715,18 @@
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="152" ht="14.25">
       <c r="A152" s="1" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>169</v>
@@ -4722,18 +4734,18 @@
       <c r="E152" s="2"/>
       <c r="F152" s="2"/>
       <c r="G152" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="153" ht="14.25">
       <c r="A153" s="1" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>169</v>
@@ -4741,18 +4753,18 @@
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
       <c r="G153" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="154" ht="14.25">
       <c r="A154" s="1" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>169</v>
@@ -4760,18 +4772,18 @@
       <c r="E154" s="2"/>
       <c r="F154" s="2"/>
       <c r="G154" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="155" ht="14.25">
       <c r="A155" s="1" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>169</v>
@@ -4779,18 +4791,18 @@
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
       <c r="G155" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="156" ht="14.25">
       <c r="A156" s="1" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>169</v>
@@ -4798,18 +4810,18 @@
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
       <c r="G156" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="157" ht="14.25">
       <c r="A157" s="1" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>169</v>
@@ -4817,18 +4829,18 @@
       <c r="E157" s="2"/>
       <c r="F157" s="2"/>
       <c r="G157" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="158" ht="14.25">
       <c r="A158" s="1" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>169</v>
@@ -4836,18 +4848,18 @@
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
       <c r="G158" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="159" ht="14.25">
       <c r="A159" s="1" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>169</v>
@@ -4855,18 +4867,18 @@
       <c r="E159" s="2"/>
       <c r="F159" s="2"/>
       <c r="G159" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="160" ht="14.25">
       <c r="A160" s="1" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>169</v>
@@ -4874,18 +4886,18 @@
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="161" ht="14.25">
       <c r="A161" s="1" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>169</v>
@@ -4893,18 +4905,18 @@
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="162" ht="14.25">
       <c r="A162" s="1" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>169</v>
@@ -4912,18 +4924,18 @@
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="163" ht="14.25">
       <c r="A163" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>169</v>
@@ -4931,18 +4943,18 @@
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="164" ht="14.25">
       <c r="A164" s="1" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>169</v>
@@ -4950,18 +4962,18 @@
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="165" ht="14.25">
       <c r="A165" s="1" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>169</v>
@@ -4969,18 +4981,18 @@
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="166" ht="14.25">
       <c r="A166" s="1" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>169</v>
@@ -4988,18 +5000,18 @@
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
       <c r="G166" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="167" ht="14.25">
       <c r="A167" s="1" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>169</v>
@@ -5007,18 +5019,18 @@
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
       <c r="G167" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="168" ht="14.25">
       <c r="A168" s="1" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>169</v>
@@ -5026,18 +5038,18 @@
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
       <c r="G168" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="169" ht="14.25">
       <c r="A169" s="1" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>169</v>
@@ -5045,18 +5057,18 @@
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
       <c r="G169" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="170" ht="14.25">
       <c r="A170" s="1" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>169</v>
@@ -5064,18 +5076,18 @@
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
       <c r="G170" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="171" ht="14.25">
       <c r="A171" s="1" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>169</v>
@@ -5083,18 +5095,18 @@
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
       <c r="G171" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="172" ht="14.25">
       <c r="A172" s="1" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>169</v>
@@ -5102,18 +5114,18 @@
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="173" ht="14.25">
       <c r="A173" s="1" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>169</v>
@@ -5121,18 +5133,18 @@
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
       <c r="G173" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="174" ht="14.25">
       <c r="A174" s="1" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>169</v>
@@ -5140,18 +5152,18 @@
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
       <c r="G174" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="175" ht="14.25">
       <c r="A175" s="1" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>169</v>
@@ -5159,18 +5171,18 @@
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
       <c r="G175" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="176" ht="14.25">
       <c r="A176" s="1" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>169</v>
@@ -5178,18 +5190,18 @@
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
       <c r="G176" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="177" ht="14.25">
       <c r="A177" s="1" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>169</v>
@@ -5197,18 +5209,18 @@
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
       <c r="G177" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="178" ht="14.25">
       <c r="A178" s="1" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>169</v>
@@ -5216,18 +5228,18 @@
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
       <c r="G178" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="179" ht="14.25">
       <c r="A179" s="1" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>169</v>
@@ -5235,7 +5247,7 @@
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
       <c r="G179" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="180" ht="14.25">

</xml_diff>

<commit_message>
Making progress on creating new dictionary.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -1448,7 +1448,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1464,6 +1464,9 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2055,7 +2058,7 @@
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2090,7 +2093,7 @@
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2127,7 +2130,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" ht="85.5">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2159,7 +2162,7 @@
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="2"/>
@@ -2172,7 +2175,7 @@
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2260,7 +2263,7 @@
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2412,7 +2415,7 @@
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -3412,7 +3415,7 @@
       <c r="A80" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="8" t="s">
         <v>266</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -3543,7 +3546,7 @@
       <c r="A87" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B87" s="8" t="s">
         <v>286</v>
       </c>
       <c r="C87" s="1" t="s">

</xml_diff>

<commit_message>
Made a slight formatting change.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -1448,7 +1448,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1464,9 +1464,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2058,7 +2055,7 @@
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2130,7 +2127,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" ht="85.5">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2162,7 +2159,7 @@
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="2"/>
@@ -2175,7 +2172,7 @@
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2263,7 +2260,7 @@
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2317,7 +2314,7 @@
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2328,7 +2325,7 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2336,7 +2333,7 @@
       <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2351,7 +2348,7 @@
       <c r="F21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2415,7 +2412,7 @@
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -3415,7 +3412,7 @@
       <c r="A80" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="7" t="s">
         <v>266</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -3546,7 +3543,7 @@
       <c r="A87" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="7" t="s">
         <v>286</v>
       </c>
       <c r="C87" s="1" t="s">

</xml_diff>

<commit_message>
About 2/3rds done with fixing dictionary.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -1421,7 +1421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -1429,46 +1429,34 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="3" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2314,7 +2302,7 @@
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2325,7 +2313,7 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2333,7 +2321,7 @@
       <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2348,7 +2336,7 @@
       <c r="F21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2356,7 +2344,7 @@
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -2371,7 +2359,7 @@
       <c r="F22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="5" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2395,13 +2383,13 @@
       <c r="A24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="5" t="s">
         <v>81</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2520,7 +2508,7 @@
       <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -2661,10 +2649,10 @@
       </c>
     </row>
     <row r="39" ht="28.5">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -2700,7 +2688,7 @@
       <c r="A41" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -2734,7 +2722,7 @@
       <c r="A43" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="5" t="s">
         <v>150</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -2773,7 +2761,7 @@
       <c r="A45" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="5" t="s">
         <v>158</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -2789,7 +2777,7 @@
       <c r="A46" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="5" t="s">
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -2881,7 +2869,7 @@
       <c r="A51" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="5" t="s">
         <v>174</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -2898,7 +2886,7 @@
       <c r="A52" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="5" t="s">
         <v>176</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -3055,7 +3043,7 @@
       <c r="A61" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="5" t="s">
         <v>203</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -3116,7 +3104,7 @@
       <c r="A64" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="5" t="s">
         <v>215</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -3412,7 +3400,7 @@
       <c r="A80" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="8" t="s">
         <v>266</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -3543,7 +3531,7 @@
       <c r="A87" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B87" s="8" t="s">
         <v>286</v>
       </c>
       <c r="C87" s="1" t="s">

</xml_diff>

<commit_message>
Fixing dictionary entries. Up to 83 entries.:
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -1433,7 +1433,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1447,16 +1447,13 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2344,7 +2341,7 @@
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -2359,7 +2356,7 @@
       <c r="F22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="2" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2383,13 +2380,13 @@
       <c r="A24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="2" t="s">
         <v>81</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2400,7 +2397,7 @@
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -2508,7 +2505,7 @@
       <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="2" t="s">
         <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -2649,10 +2646,10 @@
       </c>
     </row>
     <row r="39" ht="28.5">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -2688,7 +2685,7 @@
       <c r="A41" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -2722,7 +2719,7 @@
       <c r="A43" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -2761,7 +2758,7 @@
       <c r="A45" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="2" t="s">
         <v>158</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -2777,7 +2774,7 @@
       <c r="A46" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -2869,7 +2866,7 @@
       <c r="A51" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -2886,7 +2883,7 @@
       <c r="A52" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -3043,7 +3040,7 @@
       <c r="A61" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -3104,7 +3101,7 @@
       <c r="A64" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="2" t="s">
         <v>215</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -3400,7 +3397,7 @@
       <c r="A80" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -3497,7 +3494,7 @@
       <c r="A85" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="7" t="s">
         <v>282</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -3531,7 +3528,7 @@
       <c r="A87" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="6" t="s">
         <v>286</v>
       </c>
       <c r="C87" s="1" t="s">

</xml_diff>

<commit_message>
Nearly done fixing dictionary.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -3494,7 +3494,7 @@
       <c r="A85" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B85" s="2" t="s">
         <v>282</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -4082,7 +4082,7 @@
       <c r="A119" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" s="7" t="s">
         <v>369</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -4093,7 +4093,7 @@
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
-      <c r="G119" s="2" t="s">
+      <c r="G119" s="7" t="s">
         <v>371</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Had some weird glitches that I fixed. Only added a few more variables.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary.xlsx
+++ b/health_data/src/my_dictionary.xlsx
@@ -1447,13 +1447,13 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2054,6 +2054,7 @@
       <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" ht="28.5">
       <c r="A7" s="1" t="s">
@@ -2397,7 +2398,7 @@
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -3397,7 +3398,7 @@
       <c r="A80" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="7" t="s">
         <v>266</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -3528,7 +3529,7 @@
       <c r="A87" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="7" t="s">
         <v>286</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -4082,7 +4083,7 @@
       <c r="A119" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B119" s="7" t="s">
+      <c r="B119" s="2" t="s">
         <v>369</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -4093,7 +4094,7 @@
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
-      <c r="G119" s="7" t="s">
+      <c r="G119" s="2" t="s">
         <v>371</v>
       </c>
     </row>

</xml_diff>